<commit_message>
feature/DEV-6025 removed duplicate file
</commit_message>
<xml_diff>
--- a/LUSID Excel - Maintain a product in multiple currencies and share classes.xlsx
+++ b/LUSID Excel - Maintain a product in multiple currencies and share classes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GusSekhon\Dev\sample-excel\sample-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828BC380-FC79-4BA1-8E4B-C22AB66CB8BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C03C62F-A105-469B-B192-8400BED424AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="798" activeTab="3" xr2:uid="{AE1F34B8-DE16-4837-B47E-A2CAD3EC07DA}"/>
+    <workbookView xWindow="1695" yWindow="1050" windowWidth="24825" windowHeight="11250" tabRatio="798" xr2:uid="{AE1F34B8-DE16-4837-B47E-A2CAD3EC07DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="14" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="474">
   <si>
     <t>Code</t>
   </si>
@@ -1285,9 +1285,6 @@
     <t>Instrument</t>
   </si>
   <si>
-    <t>TimeVariant</t>
-  </si>
-  <si>
     <t>Perpetual</t>
   </si>
   <si>
@@ -1346,9 +1343,6 @@
   </si>
   <si>
     <t>UK_High_Growth_Equities_Fund:UKHGE_base_fund</t>
-  </si>
-  <si>
-    <t>total_circulation1</t>
   </si>
   <si>
     <t>Holding/default/SubHoldingKey:Value,Instrument/default/Name:Value,Holding/default/Units:Sum,Holding/default/Cost:Sum,Holding/default/PV:Sum</t>
@@ -2029,13 +2023,13 @@
     <xf numFmtId="4" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2059,6 +2053,335 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
+<volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <volType type="realTimeData">
+    <main first="rtdsrv.80d02c55f2694ff2a6ca43a30ce889e0">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>01d16cbc-b204-424b-aced-e680b844659c</stp>
+        <tr r="H40" s="24"/>
+        <tr r="I40" s="24"/>
+        <tr r="G34" s="24"/>
+        <tr r="I38" s="24"/>
+        <tr r="I35" s="24"/>
+        <tr r="G42" s="24"/>
+        <tr r="H35" s="24"/>
+        <tr r="H33" s="24"/>
+        <tr r="H37" s="24"/>
+        <tr r="I33" s="24"/>
+        <tr r="G43" s="24"/>
+        <tr r="G36" s="24"/>
+        <tr r="F37" s="24"/>
+        <tr r="H39" s="24"/>
+        <tr r="E41" s="24"/>
+        <tr r="F44" s="24"/>
+        <tr r="F43" s="24"/>
+        <tr r="I44" s="24"/>
+        <tr r="H42" s="24"/>
+        <tr r="I36" s="24"/>
+        <tr r="I34" s="24"/>
+        <tr r="G40" s="24"/>
+        <tr r="H34" s="24"/>
+        <tr r="H41" s="24"/>
+        <tr r="I41" s="24"/>
+        <tr r="H44" s="24"/>
+        <tr r="F42" s="24"/>
+        <tr r="H38" s="24"/>
+        <tr r="G37" s="24"/>
+        <tr r="H36" s="24"/>
+        <tr r="E38" s="24"/>
+        <tr r="E44" s="24"/>
+        <tr r="G35" s="24"/>
+        <tr r="I43" s="24"/>
+        <tr r="E43" s="24"/>
+        <tr r="F41" s="24"/>
+        <tr r="G33" s="24"/>
+        <tr r="F35" s="24"/>
+        <tr r="I42" s="24"/>
+        <tr r="E33" s="24"/>
+        <tr r="I39" s="24"/>
+        <tr r="E40" s="24"/>
+        <tr r="F33" s="24"/>
+        <tr r="E34" s="24"/>
+        <tr r="H43" s="24"/>
+        <tr r="E39" s="24"/>
+        <tr r="E35" s="24"/>
+        <tr r="I37" s="24"/>
+        <tr r="G41" s="24"/>
+        <tr r="F40" s="24"/>
+        <tr r="E37" s="24"/>
+        <tr r="F38" s="24"/>
+        <tr r="F34" s="24"/>
+        <tr r="E36" s="24"/>
+        <tr r="G39" s="24"/>
+        <tr r="F39" s="24"/>
+        <tr r="E42" s="24"/>
+        <tr r="G38" s="24"/>
+        <tr r="G44" s="24"/>
+        <tr r="F36" s="24"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.80d02c55f2694ff2a6ca43a30ce889e0">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>734827e9-ae6e-4fe3-a68f-207dc65ce9c2</stp>
+        <tr r="F56" s="16"/>
+        <tr r="E53" s="16"/>
+        <tr r="I55" s="16"/>
+        <tr r="K58" s="16"/>
+        <tr r="H59" s="16"/>
+        <tr r="J59" s="16"/>
+        <tr r="K60" s="16"/>
+        <tr r="E57" s="16"/>
+        <tr r="L57" s="16"/>
+        <tr r="E60" s="16"/>
+        <tr r="G59" s="16"/>
+        <tr r="J58" s="16"/>
+        <tr r="K61" s="16"/>
+        <tr r="F62" s="16"/>
+        <tr r="I60" s="16"/>
+        <tr r="K55" s="16"/>
+        <tr r="J52" s="16"/>
+        <tr r="K59" s="16"/>
+        <tr r="I53" s="16"/>
+        <tr r="J54" s="16"/>
+        <tr r="J53" s="16"/>
+        <tr r="H58" s="16"/>
+        <tr r="H52" s="16"/>
+        <tr r="F58" s="16"/>
+        <tr r="H60" s="16"/>
+        <tr r="L53" s="16"/>
+        <tr r="E58" s="16"/>
+        <tr r="F57" s="16"/>
+        <tr r="J55" s="16"/>
+        <tr r="E54" s="16"/>
+        <tr r="E59" s="16"/>
+        <tr r="G52" s="16"/>
+        <tr r="G55" s="16"/>
+        <tr r="I58" s="16"/>
+        <tr r="G58" s="16"/>
+        <tr r="H57" s="16"/>
+        <tr r="I62" s="16"/>
+        <tr r="G57" s="16"/>
+        <tr r="K57" s="16"/>
+        <tr r="F52" s="16"/>
+        <tr r="L58" s="16"/>
+        <tr r="G54" s="16"/>
+        <tr r="G53" s="16"/>
+        <tr r="H55" s="16"/>
+        <tr r="J62" s="16"/>
+        <tr r="E62" s="16"/>
+        <tr r="E52" s="16"/>
+        <tr r="K62" s="16"/>
+        <tr r="F55" s="16"/>
+        <tr r="I57" s="16"/>
+        <tr r="F59" s="16"/>
+        <tr r="H56" s="16"/>
+        <tr r="E55" s="16"/>
+        <tr r="K56" s="16"/>
+        <tr r="L61" s="16"/>
+        <tr r="I56" s="16"/>
+        <tr r="I52" s="16"/>
+        <tr r="H54" s="16"/>
+        <tr r="J57" s="16"/>
+        <tr r="I54" s="16"/>
+        <tr r="L62" s="16"/>
+        <tr r="I59" s="16"/>
+        <tr r="K54" s="16"/>
+        <tr r="I61" s="16"/>
+        <tr r="K52" s="16"/>
+        <tr r="L60" s="16"/>
+        <tr r="F61" s="16"/>
+        <tr r="L56" s="16"/>
+        <tr r="L54" s="16"/>
+        <tr r="H61" s="16"/>
+        <tr r="F53" s="16"/>
+        <tr r="L59" s="16"/>
+        <tr r="J56" s="16"/>
+        <tr r="G60" s="16"/>
+        <tr r="K53" s="16"/>
+        <tr r="L52" s="16"/>
+        <tr r="E61" s="16"/>
+        <tr r="H62" s="16"/>
+        <tr r="G61" s="16"/>
+        <tr r="H53" s="16"/>
+        <tr r="G56" s="16"/>
+        <tr r="J61" s="16"/>
+        <tr r="E56" s="16"/>
+        <tr r="F54" s="16"/>
+        <tr r="L55" s="16"/>
+        <tr r="G62" s="16"/>
+        <tr r="F60" s="16"/>
+        <tr r="J60" s="16"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.80d02c55f2694ff2a6ca43a30ce889e0">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>dd63dab0-b33d-46c7-9379-ac5e33152b0e</stp>
+        <tr r="I37" s="20"/>
+        <tr r="F40" s="20"/>
+        <tr r="F34" s="20"/>
+        <tr r="H41" s="20"/>
+        <tr r="E34" s="20"/>
+        <tr r="E41" s="20"/>
+        <tr r="G36" s="20"/>
+        <tr r="F37" s="20"/>
+        <tr r="I42" s="20"/>
+        <tr r="G35" s="20"/>
+        <tr r="E38" s="20"/>
+        <tr r="E43" s="20"/>
+        <tr r="F42" s="20"/>
+        <tr r="H40" s="20"/>
+        <tr r="I35" s="20"/>
+        <tr r="F38" s="20"/>
+        <tr r="F45" s="20"/>
+        <tr r="E35" s="20"/>
+        <tr r="I38" s="20"/>
+        <tr r="H34" s="20"/>
+        <tr r="I36" s="20"/>
+        <tr r="F43" s="20"/>
+        <tr r="F41" s="20"/>
+        <tr r="G39" s="20"/>
+        <tr r="G43" s="20"/>
+        <tr r="H43" s="20"/>
+        <tr r="H38" s="20"/>
+        <tr r="G38" s="20"/>
+        <tr r="I44" s="20"/>
+        <tr r="E40" s="20"/>
+        <tr r="H44" s="20"/>
+        <tr r="I43" s="20"/>
+        <tr r="G44" s="20"/>
+        <tr r="I41" s="20"/>
+        <tr r="H45" s="20"/>
+        <tr r="G34" s="20"/>
+        <tr r="H39" s="20"/>
+        <tr r="H37" s="20"/>
+        <tr r="E42" s="20"/>
+        <tr r="F35" s="20"/>
+        <tr r="G42" s="20"/>
+        <tr r="E39" s="20"/>
+        <tr r="G45" s="20"/>
+        <tr r="E44" s="20"/>
+        <tr r="G37" s="20"/>
+        <tr r="I34" s="20"/>
+        <tr r="F44" s="20"/>
+        <tr r="H36" s="20"/>
+        <tr r="E45" s="20"/>
+        <tr r="I39" s="20"/>
+        <tr r="F39" s="20"/>
+        <tr r="G40" s="20"/>
+        <tr r="I45" s="20"/>
+        <tr r="I40" s="20"/>
+        <tr r="G41" s="20"/>
+        <tr r="H35" s="20"/>
+        <tr r="E36" s="20"/>
+        <tr r="H42" s="20"/>
+        <tr r="E37" s="20"/>
+        <tr r="F36" s="20"/>
+      </tp>
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>70fbe34c-3155-4847-890f-52016bbe5273</stp>
+        <tr r="H73" s="16"/>
+        <tr r="I72" s="16"/>
+        <tr r="E72" s="16"/>
+        <tr r="L79" s="16"/>
+        <tr r="F72" s="16"/>
+        <tr r="G73" s="16"/>
+        <tr r="L80" s="16"/>
+        <tr r="L81" s="16"/>
+        <tr r="I75" s="16"/>
+        <tr r="F73" s="16"/>
+        <tr r="G71" s="16"/>
+        <tr r="G75" s="16"/>
+        <tr r="H78" s="16"/>
+        <tr r="I74" s="16"/>
+        <tr r="J80" s="16"/>
+        <tr r="J74" s="16"/>
+        <tr r="E74" s="16"/>
+        <tr r="E81" s="16"/>
+        <tr r="L77" s="16"/>
+        <tr r="H80" s="16"/>
+        <tr r="H81" s="16"/>
+        <tr r="E79" s="16"/>
+        <tr r="H75" s="16"/>
+        <tr r="L76" s="16"/>
+        <tr r="K80" s="16"/>
+        <tr r="K72" s="16"/>
+        <tr r="G77" s="16"/>
+        <tr r="H74" s="16"/>
+        <tr r="F74" s="16"/>
+        <tr r="L74" s="16"/>
+        <tr r="F76" s="16"/>
+        <tr r="G81" s="16"/>
+        <tr r="H72" s="16"/>
+        <tr r="H77" s="16"/>
+        <tr r="I78" s="16"/>
+        <tr r="E80" s="16"/>
+        <tr r="K76" s="16"/>
+        <tr r="F78" s="16"/>
+        <tr r="I71" s="16"/>
+        <tr r="F81" s="16"/>
+        <tr r="J76" s="16"/>
+        <tr r="H76" s="16"/>
+        <tr r="E76" s="16"/>
+        <tr r="I81" s="16"/>
+        <tr r="J77" s="16"/>
+        <tr r="G72" s="16"/>
+        <tr r="I77" s="16"/>
+        <tr r="E77" s="16"/>
+        <tr r="J71" s="16"/>
+        <tr r="L75" s="16"/>
+        <tr r="G74" s="16"/>
+        <tr r="G80" s="16"/>
+        <tr r="F79" s="16"/>
+        <tr r="L78" s="16"/>
+        <tr r="K77" s="16"/>
+        <tr r="L71" s="16"/>
+        <tr r="E71" s="16"/>
+        <tr r="I79" s="16"/>
+        <tr r="G79" s="16"/>
+        <tr r="I80" s="16"/>
+        <tr r="H79" s="16"/>
+        <tr r="K79" s="16"/>
+        <tr r="J72" s="16"/>
+        <tr r="K78" s="16"/>
+        <tr r="L73" s="16"/>
+        <tr r="K81" s="16"/>
+        <tr r="E78" s="16"/>
+        <tr r="K75" s="16"/>
+        <tr r="J81" s="16"/>
+        <tr r="J78" s="16"/>
+        <tr r="J73" s="16"/>
+        <tr r="F80" s="16"/>
+        <tr r="I73" s="16"/>
+        <tr r="L72" s="16"/>
+        <tr r="F75" s="16"/>
+        <tr r="K73" s="16"/>
+        <tr r="E73" s="16"/>
+        <tr r="F71" s="16"/>
+        <tr r="G76" s="16"/>
+        <tr r="E75" s="16"/>
+        <tr r="K74" s="16"/>
+        <tr r="J79" s="16"/>
+        <tr r="K71" s="16"/>
+        <tr r="G78" s="16"/>
+        <tr r="F77" s="16"/>
+        <tr r="J75" s="16"/>
+        <tr r="H71" s="16"/>
+        <tr r="I76" s="16"/>
+      </tp>
+    </main>
+  </volType>
+</volTypes>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3322,9 +3645,7 @@
   </sheetPr>
   <dimension ref="B1:O48"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4024,7 +4345,7 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="54" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="F14" s="54"/>
       <c r="G14" s="54"/>
@@ -4037,7 +4358,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="53" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="F15" s="54"/>
       <c r="G15" s="54"/>
@@ -4132,7 +4453,7 @@
       </c>
       <c r="F22" s="89">
         <f ca="1">NOW()-4</f>
-        <v>43808.419595949075</v>
+        <v>43833.39007858796</v>
       </c>
       <c r="G22" s="55"/>
       <c r="H22" s="2"/>
@@ -4237,13 +4558,13 @@
       </c>
       <c r="F26" s="49"/>
       <c r="G26" s="38" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="H26" s="109" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="I26" s="21" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J26" s="21" t="s">
         <v>371</v>
@@ -4257,13 +4578,13 @@
       </c>
       <c r="M26" s="87">
         <f ca="1">$F$22</f>
-        <v>43808.419595949075</v>
+        <v>43833.39007858796</v>
       </c>
       <c r="N26" s="50"/>
       <c r="O26" s="50"/>
       <c r="P26" s="50" t="str">
         <f ca="1">_xll.flQuotesAdd(F20,E25:O33)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Added 8 quote(s) as at time 2020-01-07 09:21:42Z</v>
       </c>
       <c r="Q26" s="2"/>
     </row>
@@ -4278,13 +4599,13 @@
       </c>
       <c r="F27" s="49"/>
       <c r="G27" s="38" t="s">
+        <v>457</v>
+      </c>
+      <c r="H27" s="38" t="s">
         <v>459</v>
       </c>
-      <c r="H27" s="38" t="s">
-        <v>461</v>
-      </c>
       <c r="I27" s="21" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J27" s="21" t="s">
         <v>371</v>
@@ -4298,7 +4619,7 @@
       </c>
       <c r="M27" s="87">
         <f t="shared" ref="M27:M33" ca="1" si="1">$F$22</f>
-        <v>43808.419595949075</v>
+        <v>43833.39007858796</v>
       </c>
       <c r="N27" s="43"/>
       <c r="O27" s="43"/>
@@ -4316,13 +4637,13 @@
       </c>
       <c r="F28" s="49"/>
       <c r="G28" s="38" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="H28" s="38" t="s">
+        <v>460</v>
+      </c>
+      <c r="I28" s="21" t="s">
         <v>462</v>
-      </c>
-      <c r="I28" s="21" t="s">
-        <v>464</v>
       </c>
       <c r="J28" s="21" t="s">
         <v>371</v>
@@ -4336,7 +4657,7 @@
       </c>
       <c r="M28" s="87">
         <f t="shared" ca="1" si="1"/>
-        <v>43808.419595949075</v>
+        <v>43833.39007858796</v>
       </c>
       <c r="N28" s="43"/>
       <c r="O28" s="43"/>
@@ -4354,13 +4675,13 @@
       </c>
       <c r="F29" s="58"/>
       <c r="G29" s="38" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="H29" s="36" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="I29" s="21" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J29" s="21" t="s">
         <v>371</v>
@@ -4374,7 +4695,7 @@
       </c>
       <c r="M29" s="87">
         <f t="shared" ca="1" si="1"/>
-        <v>43808.419595949075</v>
+        <v>43833.39007858796</v>
       </c>
       <c r="N29" s="87"/>
       <c r="O29" s="87"/>
@@ -4392,13 +4713,13 @@
       </c>
       <c r="F30" s="58"/>
       <c r="G30" s="38" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="H30" s="36" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I30" s="21" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J30" s="21" t="s">
         <v>371</v>
@@ -4412,7 +4733,7 @@
       </c>
       <c r="M30" s="87">
         <f t="shared" ca="1" si="1"/>
-        <v>43808.419595949075</v>
+        <v>43833.39007858796</v>
       </c>
       <c r="N30" s="34"/>
       <c r="O30" s="34"/>
@@ -4430,13 +4751,13 @@
       </c>
       <c r="F31" s="58"/>
       <c r="G31" s="38" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="H31" s="36" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="I31" s="21" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J31" s="21" t="s">
         <v>371</v>
@@ -4450,7 +4771,7 @@
       </c>
       <c r="M31" s="87">
         <f t="shared" ca="1" si="1"/>
-        <v>43808.419595949075</v>
+        <v>43833.39007858796</v>
       </c>
       <c r="N31" s="34"/>
       <c r="O31" s="34"/>
@@ -4468,13 +4789,13 @@
       </c>
       <c r="F32" s="58"/>
       <c r="G32" s="38" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="H32" s="36" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="I32" s="21" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J32" s="21" t="s">
         <v>371</v>
@@ -4488,7 +4809,7 @@
       </c>
       <c r="M32" s="87">
         <f t="shared" ca="1" si="1"/>
-        <v>43808.419595949075</v>
+        <v>43833.39007858796</v>
       </c>
       <c r="N32" s="34"/>
       <c r="O32" s="34"/>
@@ -4506,13 +4827,13 @@
       </c>
       <c r="F33" s="58"/>
       <c r="G33" s="38" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="H33" s="36" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="I33" s="21" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J33" s="21" t="s">
         <v>371</v>
@@ -4526,7 +4847,7 @@
       </c>
       <c r="M33" s="87">
         <f t="shared" ca="1" si="1"/>
-        <v>43808.419595949075</v>
+        <v>43833.39007858796</v>
       </c>
       <c r="N33" s="34"/>
       <c r="O33" s="34"/>
@@ -4796,7 +5117,7 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="53" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="F14" s="54"/>
       <c r="G14" s="54"/>
@@ -4808,7 +5129,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="53" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="F15" s="54"/>
       <c r="G15" s="54"/>
@@ -4834,12 +5155,12 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="54" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="F17" s="54"/>
       <c r="G17" s="54"/>
       <c r="K17" s="42" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="L17" s="11"/>
     </row>
@@ -4851,7 +5172,7 @@
       <c r="F18" s="54"/>
       <c r="G18" s="54"/>
       <c r="K18" s="42" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="L18" s="2"/>
     </row>
@@ -4860,7 +5181,7 @@
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
       <c r="E19" s="55" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="F19" s="55">
         <f>'Securitising base fund'!G50/COUNTA('Create foreign ccy portfolios'!I29:I33)</f>
@@ -4868,7 +5189,7 @@
       </c>
       <c r="G19" s="55"/>
       <c r="H19" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -4881,15 +5202,15 @@
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="55" t="s">
-        <v>475</v>
-      </c>
-      <c r="F20" s="112" t="e">
+        <v>473</v>
+      </c>
+      <c r="F20" s="110">
         <f ca="1">'Unit price calc'!E34/COUNTA('Create foreign ccy portfolios'!I29:I33)</f>
-        <v>#VALUE!</v>
+        <v>8621901.5739999991</v>
       </c>
       <c r="G20" s="55"/>
       <c r="H20" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -4909,7 +5230,7 @@
       </c>
       <c r="G21" s="55"/>
       <c r="H21" s="2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -4925,7 +5246,7 @@
       <c r="F22" s="55"/>
       <c r="G22" s="55"/>
       <c r="H22" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -4941,11 +5262,11 @@
         <v>186</v>
       </c>
       <c r="F23" s="61" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="G23" s="55"/>
       <c r="H23" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -4976,7 +5297,7 @@
       </c>
       <c r="F25" s="74">
         <f ca="1">NOW()-4</f>
-        <v>43808.419566087963</v>
+        <v>43833.390075462965</v>
       </c>
       <c r="G25" s="55" t="s">
         <v>358</v>
@@ -5286,7 +5607,7 @@
       <c r="D40" s="2"/>
       <c r="E40" s="11" t="str">
         <f ca="1">_xll.flHoldingsAdjust(F21,F23,F25,E28:M38)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Holdings set for portfolio code AUD_UKHGE_base_fund</v>
       </c>
       <c r="F40" s="55"/>
       <c r="G40" s="55"/>
@@ -6098,11 +6419,11 @@
       </c>
       <c r="L28" s="40">
         <f ca="1">NOW()-2</f>
-        <v>43810.419596527776</v>
+        <v>43835.390095023147</v>
       </c>
       <c r="M28" s="49" t="str">
         <f ca="1">_xll.flPortfoliosAddDerived(F24,E27:L28)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Portfolio with id Pension-fund in scope Production-client effective 2020-01-05T09:21:44.2100000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="N28" s="2"/>
     </row>
@@ -6433,7 +6754,7 @@
       </c>
       <c r="I50" s="75">
         <f ca="1">'Create scope and portfolio'!H29</f>
-        <v>43447.419596180553</v>
+        <v>43472.390093518516</v>
       </c>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
@@ -6465,36 +6786,36 @@
       <c r="C52" s="2"/>
       <c r="D52" s="55"/>
       <c r="E52" s="9" t="str">
-        <f t="array" aca="1" ref="E52:L62" ca="1">_xll.flHoldingsGet(F50,F51,I50)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <f t="array" ref="E52:L62" ca="1">_xll.flHoldingsGet(F50,F51,I50)</f>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F52" s="9" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G52" s="7" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H52" s="6" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I52" s="9" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J52" s="9" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K52" s="6" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L52" s="6" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
@@ -6507,35 +6828,35 @@
       </c>
       <c r="E53" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F53" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G53" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H53" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I53" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J53" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K53" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L53" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -6548,35 +6869,35 @@
       </c>
       <c r="E54" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F54" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G54" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H54" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I54" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J54" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K54" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L54" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -6589,35 +6910,35 @@
       </c>
       <c r="E55" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F55" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G55" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H55" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I55" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J55" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K55" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L55" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
@@ -6630,35 +6951,35 @@
       </c>
       <c r="E56" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F56" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G56" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H56" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I56" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J56" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K56" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L56" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
@@ -6671,35 +6992,35 @@
       </c>
       <c r="E57" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F57" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G57" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H57" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I57" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J57" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K57" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L57" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
@@ -6712,35 +7033,35 @@
       </c>
       <c r="E58" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F58" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G58" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H58" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I58" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J58" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K58" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L58" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -6753,35 +7074,35 @@
       </c>
       <c r="E59" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F59" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G59" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H59" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I59" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J59" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K59" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L59" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -6794,35 +7115,35 @@
       </c>
       <c r="E60" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F60" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G60" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H60" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I60" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J60" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K60" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L60" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
@@ -6835,35 +7156,35 @@
       </c>
       <c r="E61" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F61" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G61" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H61" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I61" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J61" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K61" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L61" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -6876,35 +7197,35 @@
       </c>
       <c r="E62" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F62" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G62" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H62" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I62" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J62" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K62" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L62" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
@@ -7001,7 +7322,7 @@
       </c>
       <c r="I69" s="75">
         <f ca="1">I50</f>
-        <v>43447.419596180553</v>
+        <v>43472.390093518516</v>
       </c>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
@@ -7033,36 +7354,36 @@
       <c r="C71" s="2"/>
       <c r="D71" s="55"/>
       <c r="E71" s="9" t="str">
-        <f t="array" aca="1" ref="E71:L81" ca="1">_xll.flHoldingsGet(F69,F70,I69)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <f t="array" ref="E71:L81" ca="1">_xll.flHoldingsGet(F69,F70,I69)</f>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F71" s="9" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G71" s="7" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H71" s="6" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I71" s="9" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J71" s="9" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K71" s="6" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L71" s="6" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
@@ -7075,35 +7396,35 @@
       </c>
       <c r="E72" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F72" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G72" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H72" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I72" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J72" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K72" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L72" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M72" s="2"/>
       <c r="N72" s="2"/>
@@ -7116,35 +7437,35 @@
       </c>
       <c r="E73" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F73" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G73" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H73" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I73" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J73" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K73" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L73" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
@@ -7157,35 +7478,35 @@
       </c>
       <c r="E74" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F74" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G74" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H74" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I74" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J74" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K74" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L74" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
@@ -7198,35 +7519,35 @@
       </c>
       <c r="E75" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F75" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G75" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H75" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I75" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J75" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K75" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L75" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
@@ -7239,35 +7560,35 @@
       </c>
       <c r="E76" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F76" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G76" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H76" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I76" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J76" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K76" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L76" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M76" s="2"/>
       <c r="N76" s="2"/>
@@ -7280,35 +7601,35 @@
       </c>
       <c r="E77" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F77" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G77" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H77" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I77" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J77" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K77" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L77" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
@@ -7321,35 +7642,35 @@
       </c>
       <c r="E78" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F78" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G78" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H78" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I78" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J78" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K78" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L78" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
@@ -7362,35 +7683,35 @@
       </c>
       <c r="E79" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F79" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G79" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H79" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I79" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J79" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K79" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L79" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
@@ -7403,35 +7724,35 @@
       </c>
       <c r="E80" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F80" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G80" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H80" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I80" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J80" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K80" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L80" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M80" s="2"/>
       <c r="N80" s="2"/>
@@ -7444,35 +7765,35 @@
       </c>
       <c r="E81" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F81" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G81" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H81" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I81" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J81" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K81" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L81" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
@@ -9054,7 +9375,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="24">
         <f ca="1">NOW()-1</f>
-        <v>43811.419596527776</v>
+        <v>43836.390095023147</v>
       </c>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
@@ -9099,7 +9420,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="24">
         <f ca="1">NOW()+1</f>
-        <v>43813.419596527776</v>
+        <v>43838.390095023147</v>
       </c>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -9195,11 +9516,11 @@
       </c>
       <c r="I28" s="39">
         <f ca="1">I23</f>
-        <v>43811.419596527776</v>
+        <v>43836.390095023147</v>
       </c>
       <c r="J28" s="39">
         <f ca="1">I25</f>
-        <v>43813.419596527776</v>
+        <v>43838.390095023147</v>
       </c>
       <c r="K28" s="27">
         <v>410000</v>
@@ -9241,11 +9562,11 @@
       </c>
       <c r="I29" s="39">
         <f ca="1">I28</f>
-        <v>43811.419596527776</v>
+        <v>43836.390095023147</v>
       </c>
       <c r="J29" s="39">
         <f ca="1">J28</f>
-        <v>43813.419596527776</v>
+        <v>43838.390095023147</v>
       </c>
       <c r="K29" s="27">
         <v>2879200</v>
@@ -9287,11 +9608,11 @@
       </c>
       <c r="I30" s="39">
         <f ca="1">I29</f>
-        <v>43811.419596527776</v>
+        <v>43836.390095023147</v>
       </c>
       <c r="J30" s="39">
         <f ca="1">J29</f>
-        <v>43813.419596527776</v>
+        <v>43838.390095023147</v>
       </c>
       <c r="K30" s="27">
         <v>669180</v>
@@ -9485,7 +9806,7 @@
       <c r="D39" s="2"/>
       <c r="E39" s="19" t="str">
         <f ca="1">_xll.flTransactionsAdd(F23,F25,E27:Q30)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2020-01-06T09:21:44.2100000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F39" s="55"/>
       <c r="G39" s="55"/>
@@ -20176,7 +20497,7 @@
       <c r="H26" s="55"/>
       <c r="I26" s="62">
         <f ca="1">NOW()-65/1440</f>
-        <v>43812.374457407408</v>
+        <v>43837.344955208333</v>
       </c>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
@@ -20221,7 +20542,7 @@
       <c r="H28" s="55"/>
       <c r="I28" s="64">
         <f ca="1">I26+2</f>
-        <v>43814.374457407408</v>
+        <v>43839.344955208333</v>
       </c>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
@@ -20318,11 +20639,11 @@
       </c>
       <c r="I31" s="65">
         <f ca="1">I26</f>
-        <v>43812.374457407408</v>
+        <v>43837.344955208333</v>
       </c>
       <c r="J31" s="39">
         <f ca="1">I28</f>
-        <v>43814.374457407408</v>
+        <v>43839.344955208333</v>
       </c>
       <c r="K31" s="27">
         <v>150000000</v>
@@ -20365,11 +20686,11 @@
       </c>
       <c r="I32" s="65">
         <f ca="1">I31</f>
-        <v>43812.374457407408</v>
+        <v>43837.344955208333</v>
       </c>
       <c r="J32" s="39">
         <f ca="1">J31</f>
-        <v>43814.374457407408</v>
+        <v>43839.344955208333</v>
       </c>
       <c r="K32" s="27">
         <v>120000000</v>
@@ -20584,7 +20905,7 @@
       <c r="D42" s="2"/>
       <c r="E42" s="51" t="str">
         <f ca="1">_xll.flTransactionsAdd(F26,F28,E30:Q34)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2020-01-07T08:16:44.1300000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F42" s="55"/>
       <c r="G42" s="55"/>
@@ -25715,7 +26036,7 @@
   </sheetPr>
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
@@ -26192,14 +26513,14 @@
         <v>345</v>
       </c>
       <c r="F29" s="58" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="G29" s="59" t="s">
         <v>357</v>
       </c>
       <c r="H29" s="74">
         <f ca="1">NOW()-365</f>
-        <v>43447.419596180553</v>
+        <v>43472.390093518516</v>
       </c>
       <c r="I29" s="59" t="s">
         <v>8</v>
@@ -26211,7 +26532,7 @@
       <c r="L29" s="15"/>
       <c r="M29" s="15" t="str">
         <f ca="1">_xll.flPortfoliosAdd(F25,E28:L29)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Entity already exists</v>
       </c>
       <c r="N29" s="17"/>
     </row>
@@ -26495,7 +26816,7 @@
   <dimension ref="B1:Y74"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26828,7 +27149,7 @@
       <c r="J24" s="43"/>
       <c r="K24" s="43" t="str">
         <f t="array" ref="K24:K32">_xll.flInstrumentsAdd(E23:J32)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>LUID_FVL71B1S</v>
       </c>
       <c r="L24" s="2"/>
       <c r="Y24" t="str">
@@ -26853,7 +27174,7 @@
       <c r="I25" s="45"/>
       <c r="J25" s="43"/>
       <c r="K25" s="43" t="str">
-        <v>#ERROR: User session not authenticated</v>
+        <v>LUID_U15233F5</v>
       </c>
       <c r="L25" s="2"/>
       <c r="Y25" t="str">
@@ -26878,7 +27199,7 @@
       <c r="I26" s="45"/>
       <c r="J26" s="43"/>
       <c r="K26" s="43" t="str">
-        <v>#ERROR: User session not authenticated</v>
+        <v>LUID_S29JE7OA</v>
       </c>
       <c r="L26" s="2"/>
       <c r="Y26" t="str">
@@ -26903,7 +27224,7 @@
       <c r="I27" s="45"/>
       <c r="J27" s="43"/>
       <c r="K27" s="43" t="str">
-        <v>#ERROR: User session not authenticated</v>
+        <v>LUID_E0FQLDV6</v>
       </c>
       <c r="L27" s="2"/>
       <c r="Y27" t="str">
@@ -26928,7 +27249,7 @@
       <c r="I28" s="45"/>
       <c r="J28" s="43"/>
       <c r="K28" s="43" t="str">
-        <v>#ERROR: User session not authenticated</v>
+        <v>LUID_6OSNPL9E</v>
       </c>
       <c r="L28" s="2"/>
       <c r="Y28" t="str">
@@ -26953,7 +27274,7 @@
       <c r="I29" s="45"/>
       <c r="J29" s="43"/>
       <c r="K29" s="43" t="str">
-        <v>#ERROR: User session not authenticated</v>
+        <v>LUID_WFWHONCP</v>
       </c>
       <c r="L29" s="2"/>
       <c r="Y29" t="str">
@@ -26978,7 +27299,7 @@
       <c r="I30" s="45"/>
       <c r="J30" s="43"/>
       <c r="K30" s="43" t="str">
-        <v>#ERROR: User session not authenticated</v>
+        <v>LUID_B3CIX5F3</v>
       </c>
       <c r="L30" s="2"/>
       <c r="Y30" t="str">
@@ -27003,7 +27324,7 @@
       <c r="I31" s="45"/>
       <c r="J31" s="43"/>
       <c r="K31" s="43" t="str">
-        <v>#ERROR: User session not authenticated</v>
+        <v>LUID_J38J7CKW</v>
       </c>
       <c r="L31" s="2"/>
       <c r="Y31" t="str">
@@ -27028,7 +27349,7 @@
       <c r="I32" s="45"/>
       <c r="J32" s="43"/>
       <c r="K32" s="43" t="str">
-        <v>#ERROR: User session not authenticated</v>
+        <v>LUID_0U2LEIHT</v>
       </c>
       <c r="L32" s="2"/>
       <c r="Y32" t="str">
@@ -27928,9 +28249,7 @@
   </sheetPr>
   <dimension ref="B1:M104"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -28162,7 +28481,7 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="54" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F19" s="54"/>
       <c r="G19" s="54"/>
@@ -28278,7 +28597,7 @@
       </c>
       <c r="F27" s="74">
         <f ca="1">NOW()-4</f>
-        <v>43808.419596180553</v>
+        <v>43833.390084606479</v>
       </c>
       <c r="G27" s="55" t="s">
         <v>358</v>
@@ -28588,7 +28907,7 @@
       <c r="D42" s="2"/>
       <c r="E42" s="11" t="str">
         <f ca="1">_xll.flHoldingsAdjust(F23,F25,F27,E30:M40)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Holdings set for portfolio code UKHGE_base_fund</v>
       </c>
       <c r="F42" s="55"/>
       <c r="G42" s="55"/>
@@ -28955,8 +29274,8 @@
   </sheetPr>
   <dimension ref="B1:Q103"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:Q41"/>
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29191,7 +29510,7 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="53" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F17" s="54"/>
       <c r="G17" s="54"/>
@@ -29210,7 +29529,7 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="54" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F18" s="54"/>
       <c r="G18" s="54"/>
@@ -29353,7 +29672,7 @@
       </c>
       <c r="F26" s="74">
         <f ca="1">NOW()-4</f>
-        <v>43808.419596180553</v>
+        <v>43833.390084606479</v>
       </c>
       <c r="G26" s="55" t="s">
         <v>358</v>
@@ -29479,13 +29798,13 @@
       </c>
       <c r="M30" s="87">
         <f ca="1">F26</f>
-        <v>43808.419596180553</v>
+        <v>43833.390084606479</v>
       </c>
       <c r="N30" s="50"/>
       <c r="O30" s="50"/>
       <c r="P30" s="50" t="str">
         <f ca="1">_xll.flQuotesAdd(F22,E29:O34)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Added 4 quote(s) as at time 2020-01-07 09:21:43Z</v>
       </c>
       <c r="Q30" s="2"/>
     </row>
@@ -29519,7 +29838,7 @@
       </c>
       <c r="M31" s="87">
         <f ca="1">M30</f>
-        <v>43808.419596180553</v>
+        <v>43833.390084606479</v>
       </c>
       <c r="N31" s="43"/>
       <c r="O31" s="43"/>
@@ -29556,7 +29875,7 @@
       </c>
       <c r="M32" s="87">
         <f ca="1">M31</f>
-        <v>43808.419596180553</v>
+        <v>43833.390084606479</v>
       </c>
       <c r="N32" s="43"/>
       <c r="O32" s="43"/>
@@ -29593,7 +29912,7 @@
       </c>
       <c r="M33" s="87">
         <f ca="1">M32</f>
-        <v>43808.419596180553</v>
+        <v>43833.390084606479</v>
       </c>
       <c r="N33" s="87"/>
       <c r="O33" s="87"/>
@@ -30089,8 +30408,8 @@
   </sheetPr>
   <dimension ref="B1:R72"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView showGridLines="0" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30298,12 +30617,12 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="54" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F15" s="54"/>
       <c r="G15" s="54"/>
       <c r="K15" s="42" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="L15" s="11"/>
       <c r="M15" s="2"/>
@@ -30315,12 +30634,12 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="53" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F16" s="54"/>
       <c r="G16" s="54"/>
       <c r="K16" s="42" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="L16" s="11"/>
       <c r="M16" s="2"/>
@@ -30498,7 +30817,7 @@
       </c>
       <c r="F27" s="89">
         <f ca="1">'Upserting market quotes'!F26</f>
-        <v>43808.419596180553</v>
+        <v>43833.390084606479</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -30606,24 +30925,24 @@
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="91" t="str">
-        <f t="array" aca="1" ref="E34:I45" ca="1">_xll.flAggregatePortfolio(F23,F25,K34:L40,L41)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <f t="array" ref="E34:I45" ca="1">_xll.flAggregatePortfolio(F23,F25,K34:L40,L41)</f>
+        <v>Sub-Holding Key</v>
       </c>
       <c r="F34" s="91" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Name</v>
       </c>
       <c r="G34" s="91" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>UnitsSum</v>
       </c>
       <c r="H34" s="91" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>CostSum</v>
       </c>
       <c r="I34" s="91" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>PVSum</v>
       </c>
       <c r="J34" s="2"/>
       <c r="K34" s="92" t="s">
@@ -30644,23 +30963,23 @@
       <c r="D35" s="2"/>
       <c r="E35" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>LusidInstrumentId=LUID_FVL71B1S/USD</v>
       </c>
       <c r="F35" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
-      </c>
-      <c r="G35" s="102" t="str">
+        <v>Amazon_Nasdaq_AMZN</v>
+      </c>
+      <c r="G35" s="102">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
-      </c>
-      <c r="H35" s="102" t="str">
+        <v>5000</v>
+      </c>
+      <c r="H35" s="102">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
-      </c>
-      <c r="I35" s="102" t="str">
+        <v>7750000</v>
+      </c>
+      <c r="I35" s="102">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>8113250</v>
       </c>
       <c r="J35" s="2"/>
       <c r="K35" s="49" t="s">
@@ -30679,23 +30998,23 @@
       <c r="D36" s="2"/>
       <c r="E36" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>LusidInstrumentId=LUID_U15233F5/USD</v>
       </c>
       <c r="F36" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
-      </c>
-      <c r="G36" s="102" t="str">
+        <v>Apple_Nasdaq_AAPL</v>
+      </c>
+      <c r="G36" s="102">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
-      </c>
-      <c r="H36" s="102" t="str">
+        <v>49567</v>
+      </c>
+      <c r="H36" s="102">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
-      </c>
-      <c r="I36" s="102" t="str">
+        <v>9417730</v>
+      </c>
+      <c r="I36" s="102">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>8466043.5999999996</v>
       </c>
       <c r="J36" s="2"/>
       <c r="K36" s="49" t="s">
@@ -30714,23 +31033,23 @@
       <c r="D37" s="2"/>
       <c r="E37" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>LusidInstrumentId=LUID_S29JE7OA/USD</v>
       </c>
       <c r="F37" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
-      </c>
-      <c r="G37" s="102" t="str">
+        <v>USTreasury_2.00_2021</v>
+      </c>
+      <c r="G37" s="102">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
-      </c>
-      <c r="H37" s="102" t="str">
+        <v>121543</v>
+      </c>
+      <c r="H37" s="102">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
-      </c>
-      <c r="I37" s="102" t="str">
+        <v>12063142.75</v>
+      </c>
+      <c r="I37" s="102">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>11911214</v>
       </c>
       <c r="J37" s="2"/>
       <c r="K37" s="49" t="s">
@@ -30738,7 +31057,7 @@
       </c>
       <c r="L37" s="99">
         <f ca="1">F27</f>
-        <v>43808.419596180553</v>
+        <v>43833.390084606479</v>
       </c>
       <c r="M37" s="100"/>
       <c r="N37" s="100"/>
@@ -30752,30 +31071,30 @@
       <c r="D38" s="2"/>
       <c r="E38" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>LusidInstrumentId=LUID_E0FQLDV6/USD</v>
       </c>
       <c r="F38" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
-      </c>
-      <c r="G38" s="102" t="str">
+        <v>USTreasury_6.875_2025</v>
+      </c>
+      <c r="G38" s="102">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
-      </c>
-      <c r="H38" s="102" t="str">
+        <v>98444</v>
+      </c>
+      <c r="H38" s="102">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
-      </c>
-      <c r="I38" s="102" t="str">
+        <v>13878635.119999999</v>
+      </c>
+      <c r="I38" s="102">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>14014487.84</v>
       </c>
       <c r="J38" s="2"/>
       <c r="K38" s="49" t="s">
         <v>385</v>
       </c>
       <c r="L38" s="97" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="M38" s="98"/>
       <c r="N38" s="98"/>
@@ -30789,30 +31108,30 @@
       <c r="D39" s="2"/>
       <c r="E39" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F39" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G39" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H39" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I39" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J39" s="2"/>
       <c r="K39" s="49" t="s">
         <v>386</v>
       </c>
       <c r="L39" s="97" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="M39" s="98"/>
       <c r="N39" s="98"/>
@@ -30826,23 +31145,23 @@
       <c r="D40" s="2"/>
       <c r="E40" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F40" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G40" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H40" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I40" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J40" s="2"/>
       <c r="K40" s="49" t="s">
@@ -30861,34 +31180,34 @@
       <c r="D41" s="2"/>
       <c r="E41" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F41" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G41" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H41" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I41" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J41" s="2"/>
       <c r="K41" s="49" t="s">
         <v>388</v>
       </c>
-      <c r="L41" s="110" t="s">
+      <c r="L41" s="111" t="s">
         <v>389</v>
       </c>
-      <c r="M41" s="111"/>
-      <c r="N41" s="111"/>
-      <c r="O41" s="111"/>
+      <c r="M41" s="112"/>
+      <c r="N41" s="112"/>
+      <c r="O41" s="112"/>
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
     </row>
@@ -30898,30 +31217,30 @@
       <c r="D42" s="2"/>
       <c r="E42" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F42" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G42" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H42" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I42" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J42" s="2"/>
       <c r="K42" s="49"/>
-      <c r="L42" s="110"/>
-      <c r="M42" s="111"/>
-      <c r="N42" s="111"/>
-      <c r="O42" s="111"/>
+      <c r="L42" s="111"/>
+      <c r="M42" s="112"/>
+      <c r="N42" s="112"/>
+      <c r="O42" s="112"/>
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
     </row>
@@ -30931,30 +31250,30 @@
       <c r="D43" s="2"/>
       <c r="E43" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F43" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G43" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H43" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I43" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J43" s="2"/>
       <c r="K43" s="49"/>
-      <c r="L43" s="110"/>
-      <c r="M43" s="111"/>
-      <c r="N43" s="111"/>
-      <c r="O43" s="111"/>
+      <c r="L43" s="111"/>
+      <c r="M43" s="112"/>
+      <c r="N43" s="112"/>
+      <c r="O43" s="112"/>
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
     </row>
@@ -30964,30 +31283,30 @@
       <c r="D44" s="2"/>
       <c r="E44" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F44" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G44" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H44" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I44" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J44" s="2"/>
       <c r="K44" s="49"/>
-      <c r="L44" s="110"/>
-      <c r="M44" s="111"/>
-      <c r="N44" s="111"/>
-      <c r="O44" s="111"/>
+      <c r="L44" s="111"/>
+      <c r="M44" s="112"/>
+      <c r="N44" s="112"/>
+      <c r="O44" s="112"/>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
     </row>
@@ -30997,30 +31316,30 @@
       <c r="D45" s="2"/>
       <c r="E45" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F45" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G45" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H45" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I45" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J45" s="2"/>
       <c r="K45" s="49"/>
-      <c r="L45" s="110"/>
-      <c r="M45" s="111"/>
-      <c r="N45" s="111"/>
-      <c r="O45" s="111"/>
+      <c r="L45" s="111"/>
+      <c r="M45" s="112"/>
+      <c r="N45" s="112"/>
+      <c r="O45" s="112"/>
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
     </row>
@@ -31035,10 +31354,10 @@
       <c r="I46" s="102"/>
       <c r="J46" s="2"/>
       <c r="K46" s="49"/>
-      <c r="L46" s="110"/>
-      <c r="M46" s="111"/>
-      <c r="N46" s="111"/>
-      <c r="O46" s="111"/>
+      <c r="L46" s="111"/>
+      <c r="M46" s="112"/>
+      <c r="N46" s="112"/>
+      <c r="O46" s="112"/>
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
     </row>
@@ -31053,10 +31372,10 @@
       <c r="I47" s="102"/>
       <c r="J47" s="2"/>
       <c r="K47" s="49"/>
-      <c r="L47" s="110"/>
-      <c r="M47" s="111"/>
-      <c r="N47" s="111"/>
-      <c r="O47" s="111"/>
+      <c r="L47" s="111"/>
+      <c r="M47" s="112"/>
+      <c r="N47" s="112"/>
+      <c r="O47" s="112"/>
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
     </row>
@@ -31071,10 +31390,10 @@
       <c r="I48" s="102"/>
       <c r="J48" s="2"/>
       <c r="K48" s="49"/>
-      <c r="L48" s="110"/>
-      <c r="M48" s="111"/>
-      <c r="N48" s="111"/>
-      <c r="O48" s="111"/>
+      <c r="L48" s="111"/>
+      <c r="M48" s="112"/>
+      <c r="N48" s="112"/>
+      <c r="O48" s="112"/>
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
     </row>
@@ -31119,8 +31438,8 @@
   </sheetPr>
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J50" sqref="J50"/>
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31322,7 +31641,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="54" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F15" s="54"/>
       <c r="G15" s="54"/>
@@ -31337,7 +31656,7 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="53" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F16" s="54"/>
       <c r="G16" s="54"/>
@@ -31352,12 +31671,12 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="53" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F17" s="54"/>
       <c r="G17" s="54"/>
       <c r="K17" s="42" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="L17" s="11"/>
       <c r="M17" s="2"/>
@@ -31372,7 +31691,7 @@
       <c r="F18" s="54"/>
       <c r="G18" s="54"/>
       <c r="K18" s="42" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
@@ -31463,7 +31782,7 @@
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -31503,7 +31822,7 @@
       </c>
       <c r="L28" s="6" t="str">
         <f t="array" ref="L28:L31">_xll.flPropertiesAdd(E28:K31)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Keys</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -31519,22 +31838,22 @@
         <v>323</v>
       </c>
       <c r="G29" s="38" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H29" s="14" t="b">
         <v>0</v>
       </c>
       <c r="I29" s="38" t="s">
+        <v>413</v>
+      </c>
+      <c r="J29" s="33" t="s">
         <v>414</v>
       </c>
-      <c r="J29" s="33" t="s">
-        <v>415</v>
-      </c>
       <c r="K29" s="43" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="L29" s="103" t="str">
-        <v>#ERROR: User session not authenticated</v>
+        <v>Entity already exists</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -31543,29 +31862,15 @@
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="11"/>
-      <c r="E30" s="38" t="s">
-        <v>396</v>
-      </c>
-      <c r="F30" s="21" t="s">
-        <v>323</v>
-      </c>
-      <c r="G30" s="38" t="s">
-        <v>418</v>
-      </c>
-      <c r="H30" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I30" s="38" t="s">
-        <v>418</v>
-      </c>
-      <c r="J30" s="33" t="s">
-        <v>415</v>
-      </c>
-      <c r="K30" s="43" t="s">
-        <v>397</v>
-      </c>
-      <c r="L30" s="103" t="str">
-        <v>#ERROR: User session not authenticated</v>
+      <c r="E30" s="38"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="43"/>
+      <c r="L30" s="103" t="e">
+        <v>#N/A</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -31581,8 +31886,8 @@
       <c r="I31" s="38"/>
       <c r="J31" s="33"/>
       <c r="K31" s="43"/>
-      <c r="L31" s="104" t="str">
-        <v>#ERROR: User session not authenticated</v>
+      <c r="L31" s="104" t="e">
+        <v>#N/A</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -31694,7 +31999,7 @@
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E39" s="11"/>
       <c r="F39" s="2"/>
@@ -31756,19 +32061,19 @@
         <v>357</v>
       </c>
       <c r="F42" s="38" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G42" s="38" t="s">
         <v>357</v>
       </c>
       <c r="H42" s="21" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I42" s="21"/>
       <c r="J42" s="33"/>
       <c r="K42" s="103" t="str">
         <f>_xll.flInstrumentsAdd(E41:J42)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>LUID_NAM9ARDX</v>
       </c>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
@@ -31796,7 +32101,7 @@
         <v>#ERROR: User session not authenticated</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
@@ -31810,16 +32115,16 @@
       <c r="B46" s="2"/>
       <c r="C46" s="11"/>
       <c r="D46" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E46" s="9" t="s">
         <v>400</v>
       </c>
-      <c r="E46" s="9" t="s">
+      <c r="F46" s="7" t="s">
         <v>401</v>
       </c>
-      <c r="F46" s="7" t="s">
+      <c r="G46" s="9" t="s">
         <v>402</v>
-      </c>
-      <c r="G46" s="9" t="s">
-        <v>403</v>
       </c>
       <c r="H46" s="9"/>
       <c r="I46" s="6"/>
@@ -31843,7 +32148,7 @@
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -31859,16 +32164,16 @@
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E49" s="9" t="s">
         <v>400</v>
       </c>
-      <c r="E49" s="9" t="s">
+      <c r="F49" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="F49" s="9" t="s">
-        <v>402</v>
-      </c>
       <c r="G49" s="92" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="H49" s="92"/>
       <c r="I49" s="9"/>
@@ -31882,7 +32187,7 @@
         <v>1</v>
       </c>
       <c r="D50" s="38" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E50" s="38" t="s">
         <v>357</v>
@@ -31895,7 +32200,7 @@
       <c r="I50" s="105"/>
       <c r="J50" s="103" t="str">
         <f>_xll.flInstrumentPropertiesAdd(D49:G50)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>OK</v>
       </c>
       <c r="K50" s="2"/>
     </row>
@@ -32009,8 +32314,8 @@
   </sheetPr>
   <dimension ref="B1:R79"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView showGridLines="0" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P68" sqref="P68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32198,7 +32503,7 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="56" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F14" s="41"/>
       <c r="G14" s="41"/>
@@ -32214,12 +32519,12 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="54" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="F15" s="54"/>
       <c r="G15" s="54"/>
       <c r="M15" s="42" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
@@ -32229,12 +32534,12 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="53" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="F16" s="54"/>
       <c r="G16" s="54"/>
       <c r="M16" s="42" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
@@ -32406,7 +32711,7 @@
       </c>
       <c r="F27" s="89">
         <f ca="1">'Upserting market quotes'!F26</f>
-        <v>43808.419596180553</v>
+        <v>43833.390084606479</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -32494,24 +32799,24 @@
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="91" t="str">
-        <f t="array" aca="1" ref="E33:I44" ca="1">_xll.flAggregatePortfolio(F23,F25,K33:L39,L40)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <f t="array" ref="E33:I44" ca="1">_xll.flAggregatePortfolio(F23,F25,K33:L39,L40)</f>
+        <v>CostSum</v>
       </c>
       <c r="F33" s="91" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>PVSum</v>
       </c>
       <c r="G33" s="91" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Name</v>
       </c>
       <c r="H33" s="91" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I33" s="91" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J33" s="2"/>
       <c r="K33" s="92" t="s">
@@ -32530,25 +32835,25 @@
       <c r="B34" s="11"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="93" t="str">
+      <c r="E34" s="93">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
-      </c>
-      <c r="F34" s="101" t="str">
+        <v>43109507.869999997</v>
+      </c>
+      <c r="F34" s="101">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>42504995.439999998</v>
       </c>
       <c r="G34" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>UKHGE base fund</v>
       </c>
       <c r="H34" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I34" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J34" s="2"/>
       <c r="K34" s="49" t="s">
@@ -32567,23 +32872,23 @@
       <c r="D35" s="2"/>
       <c r="E35" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F35" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G35" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H35" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I35" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J35" s="2"/>
       <c r="K35" s="49" t="s">
@@ -32602,23 +32907,23 @@
       <c r="D36" s="2"/>
       <c r="E36" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F36" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G36" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H36" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I36" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J36" s="2"/>
       <c r="K36" s="49" t="s">
@@ -32626,7 +32931,7 @@
       </c>
       <c r="L36" s="99">
         <f ca="1">F27</f>
-        <v>43808.419596180553</v>
+        <v>43833.390084606479</v>
       </c>
       <c r="M36" s="100"/>
       <c r="N36" s="100"/>
@@ -32640,30 +32945,30 @@
       <c r="D37" s="2"/>
       <c r="E37" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F37" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G37" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H37" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I37" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J37" s="2"/>
       <c r="K37" s="49" t="s">
         <v>385</v>
       </c>
       <c r="L37" s="97" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="M37" s="98"/>
       <c r="N37" s="98"/>
@@ -32677,30 +32982,30 @@
       <c r="D38" s="2"/>
       <c r="E38" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F38" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G38" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H38" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I38" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J38" s="2"/>
       <c r="K38" s="49" t="s">
         <v>386</v>
       </c>
       <c r="L38" s="97" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="M38" s="98"/>
       <c r="N38" s="98"/>
@@ -32714,23 +33019,23 @@
       <c r="D39" s="2"/>
       <c r="E39" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F39" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G39" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H39" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I39" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J39" s="2"/>
       <c r="K39" s="49" t="s">
@@ -32749,34 +33054,34 @@
       <c r="D40" s="2"/>
       <c r="E40" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F40" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G40" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H40" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I40" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J40" s="2"/>
       <c r="K40" s="49" t="s">
         <v>388</v>
       </c>
-      <c r="L40" s="110" t="s">
+      <c r="L40" s="111" t="s">
         <v>389</v>
       </c>
-      <c r="M40" s="111"/>
-      <c r="N40" s="111"/>
-      <c r="O40" s="111"/>
+      <c r="M40" s="112"/>
+      <c r="N40" s="112"/>
+      <c r="O40" s="112"/>
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
     </row>
@@ -32786,30 +33091,30 @@
       <c r="D41" s="2"/>
       <c r="E41" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F41" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G41" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H41" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I41" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J41" s="2"/>
       <c r="K41" s="49"/>
-      <c r="L41" s="110"/>
-      <c r="M41" s="111"/>
-      <c r="N41" s="111"/>
-      <c r="O41" s="111"/>
+      <c r="L41" s="111"/>
+      <c r="M41" s="112"/>
+      <c r="N41" s="112"/>
+      <c r="O41" s="112"/>
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
     </row>
@@ -32819,30 +33124,30 @@
       <c r="D42" s="2"/>
       <c r="E42" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F42" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G42" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H42" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I42" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J42" s="2"/>
       <c r="K42" s="49"/>
-      <c r="L42" s="110"/>
-      <c r="M42" s="111"/>
-      <c r="N42" s="111"/>
-      <c r="O42" s="111"/>
+      <c r="L42" s="111"/>
+      <c r="M42" s="112"/>
+      <c r="N42" s="112"/>
+      <c r="O42" s="112"/>
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
     </row>
@@ -32852,30 +33157,30 @@
       <c r="D43" s="2"/>
       <c r="E43" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F43" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G43" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H43" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I43" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J43" s="2"/>
       <c r="K43" s="49"/>
-      <c r="L43" s="110"/>
-      <c r="M43" s="111"/>
-      <c r="N43" s="111"/>
-      <c r="O43" s="111"/>
+      <c r="L43" s="111"/>
+      <c r="M43" s="112"/>
+      <c r="N43" s="112"/>
+      <c r="O43" s="112"/>
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
     </row>
@@ -32885,30 +33190,30 @@
       <c r="D44" s="2"/>
       <c r="E44" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F44" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G44" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H44" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I44" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J44" s="2"/>
       <c r="K44" s="49"/>
-      <c r="L44" s="110"/>
-      <c r="M44" s="111"/>
-      <c r="N44" s="111"/>
-      <c r="O44" s="111"/>
+      <c r="L44" s="111"/>
+      <c r="M44" s="112"/>
+      <c r="N44" s="112"/>
+      <c r="O44" s="112"/>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
     </row>
@@ -32923,10 +33228,10 @@
       <c r="I45" s="102"/>
       <c r="J45" s="2"/>
       <c r="K45" s="49"/>
-      <c r="L45" s="110"/>
-      <c r="M45" s="111"/>
-      <c r="N45" s="111"/>
-      <c r="O45" s="111"/>
+      <c r="L45" s="111"/>
+      <c r="M45" s="112"/>
+      <c r="N45" s="112"/>
+      <c r="O45" s="112"/>
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
     </row>
@@ -32941,10 +33246,10 @@
       <c r="I46" s="102"/>
       <c r="J46" s="2"/>
       <c r="K46" s="49"/>
-      <c r="L46" s="110"/>
-      <c r="M46" s="111"/>
-      <c r="N46" s="111"/>
-      <c r="O46" s="111"/>
+      <c r="L46" s="111"/>
+      <c r="M46" s="112"/>
+      <c r="N46" s="112"/>
+      <c r="O46" s="112"/>
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
     </row>
@@ -32959,10 +33264,10 @@
       <c r="I47" s="102"/>
       <c r="J47" s="2"/>
       <c r="K47" s="49"/>
-      <c r="L47" s="110"/>
-      <c r="M47" s="111"/>
-      <c r="N47" s="111"/>
-      <c r="O47" s="111"/>
+      <c r="L47" s="111"/>
+      <c r="M47" s="112"/>
+      <c r="N47" s="112"/>
+      <c r="O47" s="112"/>
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
     </row>
@@ -33005,7 +33310,7 @@
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
@@ -33015,7 +33320,7 @@
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="F52" s="41"/>
       <c r="G52" s="108">
@@ -33034,12 +33339,12 @@
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F53" s="41"/>
-      <c r="G53" s="108" t="str">
+      <c r="G53" s="108">
         <f ca="1">F34</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>42504995.439999998</v>
       </c>
       <c r="M53" s="42"/>
       <c r="N53" s="2"/>
@@ -33050,12 +33355,12 @@
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="53" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="F54" s="54"/>
-      <c r="G54" s="54" t="e">
+      <c r="G54" s="54">
         <f ca="1">ROUND(G53/G52,2)</f>
-        <v>#VALUE!</v>
+        <v>1062.6199999999999</v>
       </c>
       <c r="M54" s="42"/>
       <c r="N54" s="2"/>
@@ -33100,7 +33405,7 @@
     <row r="58" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="60" spans="2:17" x14ac:dyDescent="0.25">
       <c r="E60" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="61" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -33170,7 +33475,7 @@
       </c>
       <c r="F64" s="74">
         <f ca="1">NOW()-4</f>
-        <v>43808.419595949075</v>
+        <v>43833.39007858796</v>
       </c>
       <c r="G64" s="55" t="s">
         <v>358</v>
@@ -33281,7 +33586,7 @@
       </c>
       <c r="H68" s="109" t="str">
         <f>'Securitising base fund'!K42</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>LUID_NAM9ARDX</v>
       </c>
       <c r="I68" s="21" t="s">
         <v>194</v>
@@ -33289,22 +33594,22 @@
       <c r="J68" s="21" t="s">
         <v>371</v>
       </c>
-      <c r="K68" s="33" t="e">
+      <c r="K68" s="33">
         <f ca="1">G54</f>
-        <v>#VALUE!</v>
+        <v>1062.6199999999999</v>
       </c>
       <c r="L68" s="43" t="s">
         <v>8</v>
       </c>
       <c r="M68" s="87">
         <f ca="1">F64</f>
-        <v>43808.419595949075</v>
+        <v>43833.39007858796</v>
       </c>
       <c r="N68" s="50"/>
       <c r="O68" s="50"/>
-      <c r="P68" s="50" t="str">
+      <c r="P68" s="103" t="str">
         <f ca="1">_xll.flQuotesAdd(F62,E67:O72)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Added 1 quote(s) as at time 2020-01-07 09:21:43Z</v>
       </c>
       <c r="Q68" s="2"/>
     </row>
@@ -33545,8 +33850,8 @@
   </sheetPr>
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33738,7 +34043,7 @@
       <c r="C13" s="55"/>
       <c r="D13" s="55"/>
       <c r="E13" s="56" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="F13" s="56"/>
       <c r="G13" s="56"/>
@@ -33768,7 +34073,7 @@
       <c r="C15" s="55"/>
       <c r="D15" s="55"/>
       <c r="E15" s="54" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="F15" s="54"/>
       <c r="G15" s="54"/>
@@ -33784,7 +34089,7 @@
       <c r="C16" s="55"/>
       <c r="D16" s="55"/>
       <c r="E16" s="54" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="F16" s="54"/>
       <c r="G16" s="54"/>
@@ -33800,7 +34105,7 @@
       <c r="C17" s="55"/>
       <c r="D17" s="55"/>
       <c r="E17" s="54" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="F17" s="54"/>
       <c r="G17" s="54"/>
@@ -34005,17 +34310,17 @@
         <v>1</v>
       </c>
       <c r="E29" s="59" t="s">
+        <v>440</v>
+      </c>
+      <c r="F29" s="58" t="s">
+        <v>441</v>
+      </c>
+      <c r="G29" s="59" t="s">
         <v>442</v>
-      </c>
-      <c r="F29" s="58" t="s">
-        <v>443</v>
-      </c>
-      <c r="G29" s="59" t="s">
-        <v>444</v>
       </c>
       <c r="H29" s="74">
         <f ca="1">NOW()-365</f>
-        <v>43447.419595949075</v>
+        <v>43472.39007858796</v>
       </c>
       <c r="I29" s="59" t="s">
         <v>14</v>
@@ -34025,9 +34330,9 @@
         <v>226</v>
       </c>
       <c r="L29" s="38"/>
-      <c r="M29" s="38" t="str">
+      <c r="M29" s="103" t="str">
         <f t="array" aca="1" ref="M29:M33" ca="1">_xll.flPortfoliosAdd(F25,E28:L33)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Entity already exists</v>
       </c>
       <c r="N29" s="17"/>
     </row>
@@ -34039,17 +34344,17 @@
         <v>2</v>
       </c>
       <c r="E30" s="59" t="s">
+        <v>443</v>
+      </c>
+      <c r="F30" s="58" t="s">
+        <v>444</v>
+      </c>
+      <c r="G30" s="59" t="s">
         <v>445</v>
-      </c>
-      <c r="F30" s="58" t="s">
-        <v>446</v>
-      </c>
-      <c r="G30" s="59" t="s">
-        <v>447</v>
       </c>
       <c r="H30" s="74">
         <f ca="1">NOW()-365</f>
-        <v>43447.419595949075</v>
+        <v>43472.39007858796</v>
       </c>
       <c r="I30" s="59" t="s">
         <v>69</v>
@@ -34059,9 +34364,9 @@
         <v>226</v>
       </c>
       <c r="L30" s="35"/>
-      <c r="M30" s="38" t="str">
+      <c r="M30" s="103" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Entity already exists</v>
       </c>
       <c r="N30" s="2"/>
     </row>
@@ -34073,17 +34378,17 @@
         <v>3</v>
       </c>
       <c r="E31" s="59" t="s">
+        <v>446</v>
+      </c>
+      <c r="F31" s="58" t="s">
+        <v>447</v>
+      </c>
+      <c r="G31" s="59" t="s">
         <v>448</v>
-      </c>
-      <c r="F31" s="58" t="s">
-        <v>449</v>
-      </c>
-      <c r="G31" s="59" t="s">
-        <v>450</v>
       </c>
       <c r="H31" s="74">
         <f ca="1">NOW()-365</f>
-        <v>43447.419595949075</v>
+        <v>43472.39007858796</v>
       </c>
       <c r="I31" s="59" t="s">
         <v>8</v>
@@ -34093,9 +34398,9 @@
         <v>226</v>
       </c>
       <c r="L31" s="35"/>
-      <c r="M31" s="38" t="str">
+      <c r="M31" s="103" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Entity already exists</v>
       </c>
       <c r="N31" s="2"/>
     </row>
@@ -34107,17 +34412,17 @@
         <v>4</v>
       </c>
       <c r="E32" s="59" t="s">
+        <v>449</v>
+      </c>
+      <c r="F32" s="58" t="s">
+        <v>450</v>
+      </c>
+      <c r="G32" s="59" t="s">
         <v>451</v>
-      </c>
-      <c r="F32" s="58" t="s">
-        <v>452</v>
-      </c>
-      <c r="G32" s="59" t="s">
-        <v>453</v>
       </c>
       <c r="H32" s="74">
         <f ca="1">NOW()-365</f>
-        <v>43447.419595949075</v>
+        <v>43472.39007858796</v>
       </c>
       <c r="I32" s="59" t="s">
         <v>5</v>
@@ -34127,9 +34432,9 @@
         <v>226</v>
       </c>
       <c r="L32" s="35"/>
-      <c r="M32" s="38" t="str">
+      <c r="M32" s="103" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Entity already exists</v>
       </c>
       <c r="N32" s="2"/>
     </row>
@@ -34141,17 +34446,17 @@
         <v>5</v>
       </c>
       <c r="E33" s="59" t="s">
+        <v>452</v>
+      </c>
+      <c r="F33" s="58" t="s">
+        <v>453</v>
+      </c>
+      <c r="G33" s="59" t="s">
         <v>454</v>
-      </c>
-      <c r="F33" s="58" t="s">
-        <v>455</v>
-      </c>
-      <c r="G33" s="59" t="s">
-        <v>456</v>
       </c>
       <c r="H33" s="74">
         <f ca="1">NOW()-365</f>
-        <v>43447.419595949075</v>
+        <v>43472.39007858796</v>
       </c>
       <c r="I33" s="59" t="s">
         <v>83</v>
@@ -34161,9 +34466,9 @@
         <v>226</v>
       </c>
       <c r="L33" s="35"/>
-      <c r="M33" s="38" t="str">
+      <c r="M33" s="103" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Entity already exists</v>
       </c>
       <c r="N33" s="2"/>
     </row>
@@ -34362,21 +34667,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ED7FFFC81E40E242B1541D0602C582EC" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="392b4aa86b54b1b44668db5e449e18a7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="43d77729-b3b5-43d2-8eeb-4fba98ba19cc" xmlns:ns4="bfb7c3a1-8446-4cdf-8803-34a87e3df632" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="da7639e5c2e6b11c3a3b85f93dd9e28c" ns3:_="" ns4:_="">
     <xsd:import namespace="43d77729-b3b5-43d2-8eeb-4fba98ba19cc"/>
@@ -34547,10 +34837,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{806B5E61-CB82-4E98-BB90-ED4847D7777A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EE340CE-0FB2-490C-8292-BC185D93D393}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="43d77729-b3b5-43d2-8eeb-4fba98ba19cc"/>
+    <ds:schemaRef ds:uri="bfb7c3a1-8446-4cdf-8803-34a87e3df632"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -34573,20 +34889,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EE340CE-0FB2-490C-8292-BC185D93D393}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{806B5E61-CB82-4E98-BB90-ED4847D7777A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="43d77729-b3b5-43d2-8eeb-4fba98ba19cc"/>
-    <ds:schemaRef ds:uri="bfb7c3a1-8446-4cdf-8803-34a87e3df632"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Re-merging to fix commit issues
</commit_message>
<xml_diff>
--- a/LUSID Excel - Maintain a product in multiple currencies and share classes.xlsx
+++ b/LUSID Excel - Maintain a product in multiple currencies and share classes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GusSekhon\Dev\sample-excel\sample-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828BC380-FC79-4BA1-8E4B-C22AB66CB8BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C03C62F-A105-469B-B192-8400BED424AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="798" activeTab="3" xr2:uid="{AE1F34B8-DE16-4837-B47E-A2CAD3EC07DA}"/>
+    <workbookView xWindow="1695" yWindow="1050" windowWidth="24825" windowHeight="11250" tabRatio="798" xr2:uid="{AE1F34B8-DE16-4837-B47E-A2CAD3EC07DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="14" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="474">
   <si>
     <t>Code</t>
   </si>
@@ -1285,9 +1285,6 @@
     <t>Instrument</t>
   </si>
   <si>
-    <t>TimeVariant</t>
-  </si>
-  <si>
     <t>Perpetual</t>
   </si>
   <si>
@@ -1346,9 +1343,6 @@
   </si>
   <si>
     <t>UK_High_Growth_Equities_Fund:UKHGE_base_fund</t>
-  </si>
-  <si>
-    <t>total_circulation1</t>
   </si>
   <si>
     <t>Holding/default/SubHoldingKey:Value,Instrument/default/Name:Value,Holding/default/Units:Sum,Holding/default/Cost:Sum,Holding/default/PV:Sum</t>
@@ -2029,13 +2023,13 @@
     <xf numFmtId="4" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2059,6 +2053,335 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
+<volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <volType type="realTimeData">
+    <main first="rtdsrv.80d02c55f2694ff2a6ca43a30ce889e0">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>01d16cbc-b204-424b-aced-e680b844659c</stp>
+        <tr r="H40" s="24"/>
+        <tr r="I40" s="24"/>
+        <tr r="G34" s="24"/>
+        <tr r="I38" s="24"/>
+        <tr r="I35" s="24"/>
+        <tr r="G42" s="24"/>
+        <tr r="H35" s="24"/>
+        <tr r="H33" s="24"/>
+        <tr r="H37" s="24"/>
+        <tr r="I33" s="24"/>
+        <tr r="G43" s="24"/>
+        <tr r="G36" s="24"/>
+        <tr r="F37" s="24"/>
+        <tr r="H39" s="24"/>
+        <tr r="E41" s="24"/>
+        <tr r="F44" s="24"/>
+        <tr r="F43" s="24"/>
+        <tr r="I44" s="24"/>
+        <tr r="H42" s="24"/>
+        <tr r="I36" s="24"/>
+        <tr r="I34" s="24"/>
+        <tr r="G40" s="24"/>
+        <tr r="H34" s="24"/>
+        <tr r="H41" s="24"/>
+        <tr r="I41" s="24"/>
+        <tr r="H44" s="24"/>
+        <tr r="F42" s="24"/>
+        <tr r="H38" s="24"/>
+        <tr r="G37" s="24"/>
+        <tr r="H36" s="24"/>
+        <tr r="E38" s="24"/>
+        <tr r="E44" s="24"/>
+        <tr r="G35" s="24"/>
+        <tr r="I43" s="24"/>
+        <tr r="E43" s="24"/>
+        <tr r="F41" s="24"/>
+        <tr r="G33" s="24"/>
+        <tr r="F35" s="24"/>
+        <tr r="I42" s="24"/>
+        <tr r="E33" s="24"/>
+        <tr r="I39" s="24"/>
+        <tr r="E40" s="24"/>
+        <tr r="F33" s="24"/>
+        <tr r="E34" s="24"/>
+        <tr r="H43" s="24"/>
+        <tr r="E39" s="24"/>
+        <tr r="E35" s="24"/>
+        <tr r="I37" s="24"/>
+        <tr r="G41" s="24"/>
+        <tr r="F40" s="24"/>
+        <tr r="E37" s="24"/>
+        <tr r="F38" s="24"/>
+        <tr r="F34" s="24"/>
+        <tr r="E36" s="24"/>
+        <tr r="G39" s="24"/>
+        <tr r="F39" s="24"/>
+        <tr r="E42" s="24"/>
+        <tr r="G38" s="24"/>
+        <tr r="G44" s="24"/>
+        <tr r="F36" s="24"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.80d02c55f2694ff2a6ca43a30ce889e0">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>734827e9-ae6e-4fe3-a68f-207dc65ce9c2</stp>
+        <tr r="F56" s="16"/>
+        <tr r="E53" s="16"/>
+        <tr r="I55" s="16"/>
+        <tr r="K58" s="16"/>
+        <tr r="H59" s="16"/>
+        <tr r="J59" s="16"/>
+        <tr r="K60" s="16"/>
+        <tr r="E57" s="16"/>
+        <tr r="L57" s="16"/>
+        <tr r="E60" s="16"/>
+        <tr r="G59" s="16"/>
+        <tr r="J58" s="16"/>
+        <tr r="K61" s="16"/>
+        <tr r="F62" s="16"/>
+        <tr r="I60" s="16"/>
+        <tr r="K55" s="16"/>
+        <tr r="J52" s="16"/>
+        <tr r="K59" s="16"/>
+        <tr r="I53" s="16"/>
+        <tr r="J54" s="16"/>
+        <tr r="J53" s="16"/>
+        <tr r="H58" s="16"/>
+        <tr r="H52" s="16"/>
+        <tr r="F58" s="16"/>
+        <tr r="H60" s="16"/>
+        <tr r="L53" s="16"/>
+        <tr r="E58" s="16"/>
+        <tr r="F57" s="16"/>
+        <tr r="J55" s="16"/>
+        <tr r="E54" s="16"/>
+        <tr r="E59" s="16"/>
+        <tr r="G52" s="16"/>
+        <tr r="G55" s="16"/>
+        <tr r="I58" s="16"/>
+        <tr r="G58" s="16"/>
+        <tr r="H57" s="16"/>
+        <tr r="I62" s="16"/>
+        <tr r="G57" s="16"/>
+        <tr r="K57" s="16"/>
+        <tr r="F52" s="16"/>
+        <tr r="L58" s="16"/>
+        <tr r="G54" s="16"/>
+        <tr r="G53" s="16"/>
+        <tr r="H55" s="16"/>
+        <tr r="J62" s="16"/>
+        <tr r="E62" s="16"/>
+        <tr r="E52" s="16"/>
+        <tr r="K62" s="16"/>
+        <tr r="F55" s="16"/>
+        <tr r="I57" s="16"/>
+        <tr r="F59" s="16"/>
+        <tr r="H56" s="16"/>
+        <tr r="E55" s="16"/>
+        <tr r="K56" s="16"/>
+        <tr r="L61" s="16"/>
+        <tr r="I56" s="16"/>
+        <tr r="I52" s="16"/>
+        <tr r="H54" s="16"/>
+        <tr r="J57" s="16"/>
+        <tr r="I54" s="16"/>
+        <tr r="L62" s="16"/>
+        <tr r="I59" s="16"/>
+        <tr r="K54" s="16"/>
+        <tr r="I61" s="16"/>
+        <tr r="K52" s="16"/>
+        <tr r="L60" s="16"/>
+        <tr r="F61" s="16"/>
+        <tr r="L56" s="16"/>
+        <tr r="L54" s="16"/>
+        <tr r="H61" s="16"/>
+        <tr r="F53" s="16"/>
+        <tr r="L59" s="16"/>
+        <tr r="J56" s="16"/>
+        <tr r="G60" s="16"/>
+        <tr r="K53" s="16"/>
+        <tr r="L52" s="16"/>
+        <tr r="E61" s="16"/>
+        <tr r="H62" s="16"/>
+        <tr r="G61" s="16"/>
+        <tr r="H53" s="16"/>
+        <tr r="G56" s="16"/>
+        <tr r="J61" s="16"/>
+        <tr r="E56" s="16"/>
+        <tr r="F54" s="16"/>
+        <tr r="L55" s="16"/>
+        <tr r="G62" s="16"/>
+        <tr r="F60" s="16"/>
+        <tr r="J60" s="16"/>
+      </tp>
+    </main>
+    <main first="rtdsrv.80d02c55f2694ff2a6ca43a30ce889e0">
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>dd63dab0-b33d-46c7-9379-ac5e33152b0e</stp>
+        <tr r="I37" s="20"/>
+        <tr r="F40" s="20"/>
+        <tr r="F34" s="20"/>
+        <tr r="H41" s="20"/>
+        <tr r="E34" s="20"/>
+        <tr r="E41" s="20"/>
+        <tr r="G36" s="20"/>
+        <tr r="F37" s="20"/>
+        <tr r="I42" s="20"/>
+        <tr r="G35" s="20"/>
+        <tr r="E38" s="20"/>
+        <tr r="E43" s="20"/>
+        <tr r="F42" s="20"/>
+        <tr r="H40" s="20"/>
+        <tr r="I35" s="20"/>
+        <tr r="F38" s="20"/>
+        <tr r="F45" s="20"/>
+        <tr r="E35" s="20"/>
+        <tr r="I38" s="20"/>
+        <tr r="H34" s="20"/>
+        <tr r="I36" s="20"/>
+        <tr r="F43" s="20"/>
+        <tr r="F41" s="20"/>
+        <tr r="G39" s="20"/>
+        <tr r="G43" s="20"/>
+        <tr r="H43" s="20"/>
+        <tr r="H38" s="20"/>
+        <tr r="G38" s="20"/>
+        <tr r="I44" s="20"/>
+        <tr r="E40" s="20"/>
+        <tr r="H44" s="20"/>
+        <tr r="I43" s="20"/>
+        <tr r="G44" s="20"/>
+        <tr r="I41" s="20"/>
+        <tr r="H45" s="20"/>
+        <tr r="G34" s="20"/>
+        <tr r="H39" s="20"/>
+        <tr r="H37" s="20"/>
+        <tr r="E42" s="20"/>
+        <tr r="F35" s="20"/>
+        <tr r="G42" s="20"/>
+        <tr r="E39" s="20"/>
+        <tr r="G45" s="20"/>
+        <tr r="E44" s="20"/>
+        <tr r="G37" s="20"/>
+        <tr r="I34" s="20"/>
+        <tr r="F44" s="20"/>
+        <tr r="H36" s="20"/>
+        <tr r="E45" s="20"/>
+        <tr r="I39" s="20"/>
+        <tr r="F39" s="20"/>
+        <tr r="G40" s="20"/>
+        <tr r="I45" s="20"/>
+        <tr r="I40" s="20"/>
+        <tr r="G41" s="20"/>
+        <tr r="H35" s="20"/>
+        <tr r="E36" s="20"/>
+        <tr r="H42" s="20"/>
+        <tr r="E37" s="20"/>
+        <tr r="F36" s="20"/>
+      </tp>
+      <tp>
+        <v>-1</v>
+        <stp/>
+        <stp>70fbe34c-3155-4847-890f-52016bbe5273</stp>
+        <tr r="H73" s="16"/>
+        <tr r="I72" s="16"/>
+        <tr r="E72" s="16"/>
+        <tr r="L79" s="16"/>
+        <tr r="F72" s="16"/>
+        <tr r="G73" s="16"/>
+        <tr r="L80" s="16"/>
+        <tr r="L81" s="16"/>
+        <tr r="I75" s="16"/>
+        <tr r="F73" s="16"/>
+        <tr r="G71" s="16"/>
+        <tr r="G75" s="16"/>
+        <tr r="H78" s="16"/>
+        <tr r="I74" s="16"/>
+        <tr r="J80" s="16"/>
+        <tr r="J74" s="16"/>
+        <tr r="E74" s="16"/>
+        <tr r="E81" s="16"/>
+        <tr r="L77" s="16"/>
+        <tr r="H80" s="16"/>
+        <tr r="H81" s="16"/>
+        <tr r="E79" s="16"/>
+        <tr r="H75" s="16"/>
+        <tr r="L76" s="16"/>
+        <tr r="K80" s="16"/>
+        <tr r="K72" s="16"/>
+        <tr r="G77" s="16"/>
+        <tr r="H74" s="16"/>
+        <tr r="F74" s="16"/>
+        <tr r="L74" s="16"/>
+        <tr r="F76" s="16"/>
+        <tr r="G81" s="16"/>
+        <tr r="H72" s="16"/>
+        <tr r="H77" s="16"/>
+        <tr r="I78" s="16"/>
+        <tr r="E80" s="16"/>
+        <tr r="K76" s="16"/>
+        <tr r="F78" s="16"/>
+        <tr r="I71" s="16"/>
+        <tr r="F81" s="16"/>
+        <tr r="J76" s="16"/>
+        <tr r="H76" s="16"/>
+        <tr r="E76" s="16"/>
+        <tr r="I81" s="16"/>
+        <tr r="J77" s="16"/>
+        <tr r="G72" s="16"/>
+        <tr r="I77" s="16"/>
+        <tr r="E77" s="16"/>
+        <tr r="J71" s="16"/>
+        <tr r="L75" s="16"/>
+        <tr r="G74" s="16"/>
+        <tr r="G80" s="16"/>
+        <tr r="F79" s="16"/>
+        <tr r="L78" s="16"/>
+        <tr r="K77" s="16"/>
+        <tr r="L71" s="16"/>
+        <tr r="E71" s="16"/>
+        <tr r="I79" s="16"/>
+        <tr r="G79" s="16"/>
+        <tr r="I80" s="16"/>
+        <tr r="H79" s="16"/>
+        <tr r="K79" s="16"/>
+        <tr r="J72" s="16"/>
+        <tr r="K78" s="16"/>
+        <tr r="L73" s="16"/>
+        <tr r="K81" s="16"/>
+        <tr r="E78" s="16"/>
+        <tr r="K75" s="16"/>
+        <tr r="J81" s="16"/>
+        <tr r="J78" s="16"/>
+        <tr r="J73" s="16"/>
+        <tr r="F80" s="16"/>
+        <tr r="I73" s="16"/>
+        <tr r="L72" s="16"/>
+        <tr r="F75" s="16"/>
+        <tr r="K73" s="16"/>
+        <tr r="E73" s="16"/>
+        <tr r="F71" s="16"/>
+        <tr r="G76" s="16"/>
+        <tr r="E75" s="16"/>
+        <tr r="K74" s="16"/>
+        <tr r="J79" s="16"/>
+        <tr r="K71" s="16"/>
+        <tr r="G78" s="16"/>
+        <tr r="F77" s="16"/>
+        <tr r="J75" s="16"/>
+        <tr r="H71" s="16"/>
+        <tr r="I76" s="16"/>
+      </tp>
+    </main>
+  </volType>
+</volTypes>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3322,9 +3645,7 @@
   </sheetPr>
   <dimension ref="B1:O48"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4024,7 +4345,7 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="54" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="F14" s="54"/>
       <c r="G14" s="54"/>
@@ -4037,7 +4358,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="53" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="F15" s="54"/>
       <c r="G15" s="54"/>
@@ -4132,7 +4453,7 @@
       </c>
       <c r="F22" s="89">
         <f ca="1">NOW()-4</f>
-        <v>43808.419595949075</v>
+        <v>43833.39007858796</v>
       </c>
       <c r="G22" s="55"/>
       <c r="H22" s="2"/>
@@ -4237,13 +4558,13 @@
       </c>
       <c r="F26" s="49"/>
       <c r="G26" s="38" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="H26" s="109" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="I26" s="21" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J26" s="21" t="s">
         <v>371</v>
@@ -4257,13 +4578,13 @@
       </c>
       <c r="M26" s="87">
         <f ca="1">$F$22</f>
-        <v>43808.419595949075</v>
+        <v>43833.39007858796</v>
       </c>
       <c r="N26" s="50"/>
       <c r="O26" s="50"/>
       <c r="P26" s="50" t="str">
         <f ca="1">_xll.flQuotesAdd(F20,E25:O33)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Added 8 quote(s) as at time 2020-01-07 09:21:42Z</v>
       </c>
       <c r="Q26" s="2"/>
     </row>
@@ -4278,13 +4599,13 @@
       </c>
       <c r="F27" s="49"/>
       <c r="G27" s="38" t="s">
+        <v>457</v>
+      </c>
+      <c r="H27" s="38" t="s">
         <v>459</v>
       </c>
-      <c r="H27" s="38" t="s">
-        <v>461</v>
-      </c>
       <c r="I27" s="21" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J27" s="21" t="s">
         <v>371</v>
@@ -4298,7 +4619,7 @@
       </c>
       <c r="M27" s="87">
         <f t="shared" ref="M27:M33" ca="1" si="1">$F$22</f>
-        <v>43808.419595949075</v>
+        <v>43833.39007858796</v>
       </c>
       <c r="N27" s="43"/>
       <c r="O27" s="43"/>
@@ -4316,13 +4637,13 @@
       </c>
       <c r="F28" s="49"/>
       <c r="G28" s="38" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="H28" s="38" t="s">
+        <v>460</v>
+      </c>
+      <c r="I28" s="21" t="s">
         <v>462</v>
-      </c>
-      <c r="I28" s="21" t="s">
-        <v>464</v>
       </c>
       <c r="J28" s="21" t="s">
         <v>371</v>
@@ -4336,7 +4657,7 @@
       </c>
       <c r="M28" s="87">
         <f t="shared" ca="1" si="1"/>
-        <v>43808.419595949075</v>
+        <v>43833.39007858796</v>
       </c>
       <c r="N28" s="43"/>
       <c r="O28" s="43"/>
@@ -4354,13 +4675,13 @@
       </c>
       <c r="F29" s="58"/>
       <c r="G29" s="38" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="H29" s="36" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="I29" s="21" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J29" s="21" t="s">
         <v>371</v>
@@ -4374,7 +4695,7 @@
       </c>
       <c r="M29" s="87">
         <f t="shared" ca="1" si="1"/>
-        <v>43808.419595949075</v>
+        <v>43833.39007858796</v>
       </c>
       <c r="N29" s="87"/>
       <c r="O29" s="87"/>
@@ -4392,13 +4713,13 @@
       </c>
       <c r="F30" s="58"/>
       <c r="G30" s="38" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="H30" s="36" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I30" s="21" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J30" s="21" t="s">
         <v>371</v>
@@ -4412,7 +4733,7 @@
       </c>
       <c r="M30" s="87">
         <f t="shared" ca="1" si="1"/>
-        <v>43808.419595949075</v>
+        <v>43833.39007858796</v>
       </c>
       <c r="N30" s="34"/>
       <c r="O30" s="34"/>
@@ -4430,13 +4751,13 @@
       </c>
       <c r="F31" s="58"/>
       <c r="G31" s="38" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="H31" s="36" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="I31" s="21" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J31" s="21" t="s">
         <v>371</v>
@@ -4450,7 +4771,7 @@
       </c>
       <c r="M31" s="87">
         <f t="shared" ca="1" si="1"/>
-        <v>43808.419595949075</v>
+        <v>43833.39007858796</v>
       </c>
       <c r="N31" s="34"/>
       <c r="O31" s="34"/>
@@ -4468,13 +4789,13 @@
       </c>
       <c r="F32" s="58"/>
       <c r="G32" s="38" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="H32" s="36" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="I32" s="21" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J32" s="21" t="s">
         <v>371</v>
@@ -4488,7 +4809,7 @@
       </c>
       <c r="M32" s="87">
         <f t="shared" ca="1" si="1"/>
-        <v>43808.419595949075</v>
+        <v>43833.39007858796</v>
       </c>
       <c r="N32" s="34"/>
       <c r="O32" s="34"/>
@@ -4506,13 +4827,13 @@
       </c>
       <c r="F33" s="58"/>
       <c r="G33" s="38" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="H33" s="36" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="I33" s="21" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="J33" s="21" t="s">
         <v>371</v>
@@ -4526,7 +4847,7 @@
       </c>
       <c r="M33" s="87">
         <f t="shared" ca="1" si="1"/>
-        <v>43808.419595949075</v>
+        <v>43833.39007858796</v>
       </c>
       <c r="N33" s="34"/>
       <c r="O33" s="34"/>
@@ -4796,7 +5117,7 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="53" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="F14" s="54"/>
       <c r="G14" s="54"/>
@@ -4808,7 +5129,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="53" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="F15" s="54"/>
       <c r="G15" s="54"/>
@@ -4834,12 +5155,12 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="54" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="F17" s="54"/>
       <c r="G17" s="54"/>
       <c r="K17" s="42" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="L17" s="11"/>
     </row>
@@ -4851,7 +5172,7 @@
       <c r="F18" s="54"/>
       <c r="G18" s="54"/>
       <c r="K18" s="42" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="L18" s="2"/>
     </row>
@@ -4860,7 +5181,7 @@
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
       <c r="E19" s="55" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="F19" s="55">
         <f>'Securitising base fund'!G50/COUNTA('Create foreign ccy portfolios'!I29:I33)</f>
@@ -4868,7 +5189,7 @@
       </c>
       <c r="G19" s="55"/>
       <c r="H19" s="2" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -4881,15 +5202,15 @@
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="55" t="s">
-        <v>475</v>
-      </c>
-      <c r="F20" s="112" t="e">
+        <v>473</v>
+      </c>
+      <c r="F20" s="110">
         <f ca="1">'Unit price calc'!E34/COUNTA('Create foreign ccy portfolios'!I29:I33)</f>
-        <v>#VALUE!</v>
+        <v>8621901.5739999991</v>
       </c>
       <c r="G20" s="55"/>
       <c r="H20" s="2" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -4909,7 +5230,7 @@
       </c>
       <c r="G21" s="55"/>
       <c r="H21" s="2" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
@@ -4925,7 +5246,7 @@
       <c r="F22" s="55"/>
       <c r="G22" s="55"/>
       <c r="H22" s="2" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
@@ -4941,11 +5262,11 @@
         <v>186</v>
       </c>
       <c r="F23" s="61" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="G23" s="55"/>
       <c r="H23" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
@@ -4976,7 +5297,7 @@
       </c>
       <c r="F25" s="74">
         <f ca="1">NOW()-4</f>
-        <v>43808.419566087963</v>
+        <v>43833.390075462965</v>
       </c>
       <c r="G25" s="55" t="s">
         <v>358</v>
@@ -5286,7 +5607,7 @@
       <c r="D40" s="2"/>
       <c r="E40" s="11" t="str">
         <f ca="1">_xll.flHoldingsAdjust(F21,F23,F25,E28:M38)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Holdings set for portfolio code AUD_UKHGE_base_fund</v>
       </c>
       <c r="F40" s="55"/>
       <c r="G40" s="55"/>
@@ -6098,11 +6419,11 @@
       </c>
       <c r="L28" s="40">
         <f ca="1">NOW()-2</f>
-        <v>43810.419596527776</v>
+        <v>43835.390095023147</v>
       </c>
       <c r="M28" s="49" t="str">
         <f ca="1">_xll.flPortfoliosAddDerived(F24,E27:L28)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Portfolio with id Pension-fund in scope Production-client effective 2020-01-05T09:21:44.2100000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="N28" s="2"/>
     </row>
@@ -6433,7 +6754,7 @@
       </c>
       <c r="I50" s="75">
         <f ca="1">'Create scope and portfolio'!H29</f>
-        <v>43447.419596180553</v>
+        <v>43472.390093518516</v>
       </c>
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
@@ -6465,36 +6786,36 @@
       <c r="C52" s="2"/>
       <c r="D52" s="55"/>
       <c r="E52" s="9" t="str">
-        <f t="array" aca="1" ref="E52:L62" ca="1">_xll.flHoldingsGet(F50,F51,I50)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <f t="array" ref="E52:L62" ca="1">_xll.flHoldingsGet(F50,F51,I50)</f>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F52" s="9" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G52" s="7" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H52" s="6" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I52" s="9" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J52" s="9" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K52" s="6" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L52" s="6" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
@@ -6507,35 +6828,35 @@
       </c>
       <c r="E53" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F53" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G53" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H53" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I53" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J53" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K53" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L53" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -6548,35 +6869,35 @@
       </c>
       <c r="E54" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F54" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G54" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H54" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I54" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J54" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K54" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L54" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -6589,35 +6910,35 @@
       </c>
       <c r="E55" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F55" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G55" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H55" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I55" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J55" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K55" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L55" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
@@ -6630,35 +6951,35 @@
       </c>
       <c r="E56" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F56" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G56" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H56" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I56" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J56" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K56" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L56" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
@@ -6671,35 +6992,35 @@
       </c>
       <c r="E57" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F57" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G57" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H57" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I57" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J57" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K57" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L57" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M57" s="2"/>
       <c r="N57" s="2"/>
@@ -6712,35 +7033,35 @@
       </c>
       <c r="E58" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F58" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G58" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H58" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I58" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J58" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K58" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L58" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -6753,35 +7074,35 @@
       </c>
       <c r="E59" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F59" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G59" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H59" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I59" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J59" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K59" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L59" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M59" s="2"/>
       <c r="N59" s="2"/>
@@ -6794,35 +7115,35 @@
       </c>
       <c r="E60" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F60" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G60" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H60" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I60" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J60" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K60" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L60" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M60" s="2"/>
       <c r="N60" s="2"/>
@@ -6835,35 +7156,35 @@
       </c>
       <c r="E61" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F61" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G61" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H61" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I61" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J61" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K61" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L61" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M61" s="2"/>
       <c r="N61" s="2"/>
@@ -6876,35 +7197,35 @@
       </c>
       <c r="E62" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F62" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G62" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H62" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I62" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J62" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K62" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L62" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
@@ -7001,7 +7322,7 @@
       </c>
       <c r="I69" s="75">
         <f ca="1">I50</f>
-        <v>43447.419596180553</v>
+        <v>43472.390093518516</v>
       </c>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
@@ -7033,36 +7354,36 @@
       <c r="C71" s="2"/>
       <c r="D71" s="55"/>
       <c r="E71" s="9" t="str">
-        <f t="array" aca="1" ref="E71:L81" ca="1">_xll.flHoldingsGet(F69,F70,I69)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <f t="array" ref="E71:L81" ca="1">_xll.flHoldingsGet(F69,F70,I69)</f>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F71" s="9" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G71" s="7" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H71" s="6" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I71" s="9" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J71" s="9" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K71" s="6" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L71" s="6" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M71" s="2"/>
       <c r="N71" s="2"/>
@@ -7075,35 +7396,35 @@
       </c>
       <c r="E72" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F72" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G72" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H72" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I72" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J72" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K72" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L72" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M72" s="2"/>
       <c r="N72" s="2"/>
@@ -7116,35 +7437,35 @@
       </c>
       <c r="E73" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F73" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G73" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H73" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I73" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J73" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K73" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L73" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
@@ -7157,35 +7478,35 @@
       </c>
       <c r="E74" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F74" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G74" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H74" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I74" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J74" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K74" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L74" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
@@ -7198,35 +7519,35 @@
       </c>
       <c r="E75" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F75" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G75" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H75" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I75" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J75" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K75" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L75" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
@@ -7239,35 +7560,35 @@
       </c>
       <c r="E76" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F76" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G76" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H76" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I76" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J76" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K76" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L76" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M76" s="2"/>
       <c r="N76" s="2"/>
@@ -7280,35 +7601,35 @@
       </c>
       <c r="E77" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F77" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G77" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H77" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I77" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J77" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K77" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L77" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M77" s="2"/>
       <c r="N77" s="2"/>
@@ -7321,35 +7642,35 @@
       </c>
       <c r="E78" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F78" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G78" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H78" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I78" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J78" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K78" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L78" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M78" s="2"/>
       <c r="N78" s="2"/>
@@ -7362,35 +7683,35 @@
       </c>
       <c r="E79" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F79" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G79" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H79" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I79" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J79" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K79" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L79" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M79" s="2"/>
       <c r="N79" s="2"/>
@@ -7403,35 +7724,35 @@
       </c>
       <c r="E80" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F80" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G80" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H80" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I80" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J80" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K80" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L80" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M80" s="2"/>
       <c r="N80" s="2"/>
@@ -7444,35 +7765,35 @@
       </c>
       <c r="E81" s="59" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F81" s="58" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="G81" s="76" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="H81" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="I81" s="77" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="J81" s="33" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="K81" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="L81" s="26" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2019-01-07T09:21:44.0800000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
@@ -9054,7 +9375,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="24">
         <f ca="1">NOW()-1</f>
-        <v>43811.419596527776</v>
+        <v>43836.390095023147</v>
       </c>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
@@ -9099,7 +9420,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="24">
         <f ca="1">NOW()+1</f>
-        <v>43813.419596527776</v>
+        <v>43838.390095023147</v>
       </c>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
@@ -9195,11 +9516,11 @@
       </c>
       <c r="I28" s="39">
         <f ca="1">I23</f>
-        <v>43811.419596527776</v>
+        <v>43836.390095023147</v>
       </c>
       <c r="J28" s="39">
         <f ca="1">I25</f>
-        <v>43813.419596527776</v>
+        <v>43838.390095023147</v>
       </c>
       <c r="K28" s="27">
         <v>410000</v>
@@ -9241,11 +9562,11 @@
       </c>
       <c r="I29" s="39">
         <f ca="1">I28</f>
-        <v>43811.419596527776</v>
+        <v>43836.390095023147</v>
       </c>
       <c r="J29" s="39">
         <f ca="1">J28</f>
-        <v>43813.419596527776</v>
+        <v>43838.390095023147</v>
       </c>
       <c r="K29" s="27">
         <v>2879200</v>
@@ -9287,11 +9608,11 @@
       </c>
       <c r="I30" s="39">
         <f ca="1">I29</f>
-        <v>43811.419596527776</v>
+        <v>43836.390095023147</v>
       </c>
       <c r="J30" s="39">
         <f ca="1">J29</f>
-        <v>43813.419596527776</v>
+        <v>43838.390095023147</v>
       </c>
       <c r="K30" s="27">
         <v>669180</v>
@@ -9485,7 +9806,7 @@
       <c r="D39" s="2"/>
       <c r="E39" s="19" t="str">
         <f ca="1">_xll.flTransactionsAdd(F23,F25,E27:Q30)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Production-client effective 2020-01-06T09:21:44.2100000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F39" s="55"/>
       <c r="G39" s="55"/>
@@ -20176,7 +20497,7 @@
       <c r="H26" s="55"/>
       <c r="I26" s="62">
         <f ca="1">NOW()-65/1440</f>
-        <v>43812.374457407408</v>
+        <v>43837.344955208333</v>
       </c>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
@@ -20221,7 +20542,7 @@
       <c r="H28" s="55"/>
       <c r="I28" s="64">
         <f ca="1">I26+2</f>
-        <v>43814.374457407408</v>
+        <v>43839.344955208333</v>
       </c>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
@@ -20318,11 +20639,11 @@
       </c>
       <c r="I31" s="65">
         <f ca="1">I26</f>
-        <v>43812.374457407408</v>
+        <v>43837.344955208333</v>
       </c>
       <c r="J31" s="39">
         <f ca="1">I28</f>
-        <v>43814.374457407408</v>
+        <v>43839.344955208333</v>
       </c>
       <c r="K31" s="27">
         <v>150000000</v>
@@ -20365,11 +20686,11 @@
       </c>
       <c r="I32" s="65">
         <f ca="1">I31</f>
-        <v>43812.374457407408</v>
+        <v>43837.344955208333</v>
       </c>
       <c r="J32" s="39">
         <f ca="1">J31</f>
-        <v>43814.374457407408</v>
+        <v>43839.344955208333</v>
       </c>
       <c r="K32" s="27">
         <v>120000000</v>
@@ -20584,7 +20905,7 @@
       <c r="D42" s="2"/>
       <c r="E42" s="51" t="str">
         <f ca="1">_xll.flTransactionsAdd(F26,F28,E30:Q34)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>#ERROR: Portfolio with id Pension-fund in scope Test-client effective 2020-01-07T08:16:44.1300000+00:00, AsAt=2020-01-07T09:21:43.5364140+00:00 does not exist.</v>
       </c>
       <c r="F42" s="55"/>
       <c r="G42" s="55"/>
@@ -25715,7 +26036,7 @@
   </sheetPr>
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
@@ -26192,14 +26513,14 @@
         <v>345</v>
       </c>
       <c r="F29" s="58" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="G29" s="59" t="s">
         <v>357</v>
       </c>
       <c r="H29" s="74">
         <f ca="1">NOW()-365</f>
-        <v>43447.419596180553</v>
+        <v>43472.390093518516</v>
       </c>
       <c r="I29" s="59" t="s">
         <v>8</v>
@@ -26211,7 +26532,7 @@
       <c r="L29" s="15"/>
       <c r="M29" s="15" t="str">
         <f ca="1">_xll.flPortfoliosAdd(F25,E28:L29)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Entity already exists</v>
       </c>
       <c r="N29" s="17"/>
     </row>
@@ -26495,7 +26816,7 @@
   <dimension ref="B1:Y74"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26828,7 +27149,7 @@
       <c r="J24" s="43"/>
       <c r="K24" s="43" t="str">
         <f t="array" ref="K24:K32">_xll.flInstrumentsAdd(E23:J32)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>LUID_FVL71B1S</v>
       </c>
       <c r="L24" s="2"/>
       <c r="Y24" t="str">
@@ -26853,7 +27174,7 @@
       <c r="I25" s="45"/>
       <c r="J25" s="43"/>
       <c r="K25" s="43" t="str">
-        <v>#ERROR: User session not authenticated</v>
+        <v>LUID_U15233F5</v>
       </c>
       <c r="L25" s="2"/>
       <c r="Y25" t="str">
@@ -26878,7 +27199,7 @@
       <c r="I26" s="45"/>
       <c r="J26" s="43"/>
       <c r="K26" s="43" t="str">
-        <v>#ERROR: User session not authenticated</v>
+        <v>LUID_S29JE7OA</v>
       </c>
       <c r="L26" s="2"/>
       <c r="Y26" t="str">
@@ -26903,7 +27224,7 @@
       <c r="I27" s="45"/>
       <c r="J27" s="43"/>
       <c r="K27" s="43" t="str">
-        <v>#ERROR: User session not authenticated</v>
+        <v>LUID_E0FQLDV6</v>
       </c>
       <c r="L27" s="2"/>
       <c r="Y27" t="str">
@@ -26928,7 +27249,7 @@
       <c r="I28" s="45"/>
       <c r="J28" s="43"/>
       <c r="K28" s="43" t="str">
-        <v>#ERROR: User session not authenticated</v>
+        <v>LUID_6OSNPL9E</v>
       </c>
       <c r="L28" s="2"/>
       <c r="Y28" t="str">
@@ -26953,7 +27274,7 @@
       <c r="I29" s="45"/>
       <c r="J29" s="43"/>
       <c r="K29" s="43" t="str">
-        <v>#ERROR: User session not authenticated</v>
+        <v>LUID_WFWHONCP</v>
       </c>
       <c r="L29" s="2"/>
       <c r="Y29" t="str">
@@ -26978,7 +27299,7 @@
       <c r="I30" s="45"/>
       <c r="J30" s="43"/>
       <c r="K30" s="43" t="str">
-        <v>#ERROR: User session not authenticated</v>
+        <v>LUID_B3CIX5F3</v>
       </c>
       <c r="L30" s="2"/>
       <c r="Y30" t="str">
@@ -27003,7 +27324,7 @@
       <c r="I31" s="45"/>
       <c r="J31" s="43"/>
       <c r="K31" s="43" t="str">
-        <v>#ERROR: User session not authenticated</v>
+        <v>LUID_J38J7CKW</v>
       </c>
       <c r="L31" s="2"/>
       <c r="Y31" t="str">
@@ -27028,7 +27349,7 @@
       <c r="I32" s="45"/>
       <c r="J32" s="43"/>
       <c r="K32" s="43" t="str">
-        <v>#ERROR: User session not authenticated</v>
+        <v>LUID_0U2LEIHT</v>
       </c>
       <c r="L32" s="2"/>
       <c r="Y32" t="str">
@@ -27928,9 +28249,7 @@
   </sheetPr>
   <dimension ref="B1:M104"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
-    </sheetView>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -28162,7 +28481,7 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="54" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F19" s="54"/>
       <c r="G19" s="54"/>
@@ -28278,7 +28597,7 @@
       </c>
       <c r="F27" s="74">
         <f ca="1">NOW()-4</f>
-        <v>43808.419596180553</v>
+        <v>43833.390084606479</v>
       </c>
       <c r="G27" s="55" t="s">
         <v>358</v>
@@ -28588,7 +28907,7 @@
       <c r="D42" s="2"/>
       <c r="E42" s="11" t="str">
         <f ca="1">_xll.flHoldingsAdjust(F23,F25,F27,E30:M40)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Holdings set for portfolio code UKHGE_base_fund</v>
       </c>
       <c r="F42" s="55"/>
       <c r="G42" s="55"/>
@@ -28955,8 +29274,8 @@
   </sheetPr>
   <dimension ref="B1:Q103"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:Q41"/>
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29191,7 +29510,7 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="53" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="F17" s="54"/>
       <c r="G17" s="54"/>
@@ -29210,7 +29529,7 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="54" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F18" s="54"/>
       <c r="G18" s="54"/>
@@ -29353,7 +29672,7 @@
       </c>
       <c r="F26" s="74">
         <f ca="1">NOW()-4</f>
-        <v>43808.419596180553</v>
+        <v>43833.390084606479</v>
       </c>
       <c r="G26" s="55" t="s">
         <v>358</v>
@@ -29479,13 +29798,13 @@
       </c>
       <c r="M30" s="87">
         <f ca="1">F26</f>
-        <v>43808.419596180553</v>
+        <v>43833.390084606479</v>
       </c>
       <c r="N30" s="50"/>
       <c r="O30" s="50"/>
       <c r="P30" s="50" t="str">
         <f ca="1">_xll.flQuotesAdd(F22,E29:O34)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Added 4 quote(s) as at time 2020-01-07 09:21:43Z</v>
       </c>
       <c r="Q30" s="2"/>
     </row>
@@ -29519,7 +29838,7 @@
       </c>
       <c r="M31" s="87">
         <f ca="1">M30</f>
-        <v>43808.419596180553</v>
+        <v>43833.390084606479</v>
       </c>
       <c r="N31" s="43"/>
       <c r="O31" s="43"/>
@@ -29556,7 +29875,7 @@
       </c>
       <c r="M32" s="87">
         <f ca="1">M31</f>
-        <v>43808.419596180553</v>
+        <v>43833.390084606479</v>
       </c>
       <c r="N32" s="43"/>
       <c r="O32" s="43"/>
@@ -29593,7 +29912,7 @@
       </c>
       <c r="M33" s="87">
         <f ca="1">M32</f>
-        <v>43808.419596180553</v>
+        <v>43833.390084606479</v>
       </c>
       <c r="N33" s="87"/>
       <c r="O33" s="87"/>
@@ -30089,8 +30408,8 @@
   </sheetPr>
   <dimension ref="B1:R72"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView showGridLines="0" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30298,12 +30617,12 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="54" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F15" s="54"/>
       <c r="G15" s="54"/>
       <c r="K15" s="42" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="L15" s="11"/>
       <c r="M15" s="2"/>
@@ -30315,12 +30634,12 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="53" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F16" s="54"/>
       <c r="G16" s="54"/>
       <c r="K16" s="42" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="L16" s="11"/>
       <c r="M16" s="2"/>
@@ -30498,7 +30817,7 @@
       </c>
       <c r="F27" s="89">
         <f ca="1">'Upserting market quotes'!F26</f>
-        <v>43808.419596180553</v>
+        <v>43833.390084606479</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -30606,24 +30925,24 @@
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="91" t="str">
-        <f t="array" aca="1" ref="E34:I45" ca="1">_xll.flAggregatePortfolio(F23,F25,K34:L40,L41)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <f t="array" ref="E34:I45" ca="1">_xll.flAggregatePortfolio(F23,F25,K34:L40,L41)</f>
+        <v>Sub-Holding Key</v>
       </c>
       <c r="F34" s="91" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Name</v>
       </c>
       <c r="G34" s="91" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>UnitsSum</v>
       </c>
       <c r="H34" s="91" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>CostSum</v>
       </c>
       <c r="I34" s="91" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>PVSum</v>
       </c>
       <c r="J34" s="2"/>
       <c r="K34" s="92" t="s">
@@ -30644,23 +30963,23 @@
       <c r="D35" s="2"/>
       <c r="E35" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>LusidInstrumentId=LUID_FVL71B1S/USD</v>
       </c>
       <c r="F35" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
-      </c>
-      <c r="G35" s="102" t="str">
+        <v>Amazon_Nasdaq_AMZN</v>
+      </c>
+      <c r="G35" s="102">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
-      </c>
-      <c r="H35" s="102" t="str">
+        <v>5000</v>
+      </c>
+      <c r="H35" s="102">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
-      </c>
-      <c r="I35" s="102" t="str">
+        <v>7750000</v>
+      </c>
+      <c r="I35" s="102">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>8113250</v>
       </c>
       <c r="J35" s="2"/>
       <c r="K35" s="49" t="s">
@@ -30679,23 +30998,23 @@
       <c r="D36" s="2"/>
       <c r="E36" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>LusidInstrumentId=LUID_U15233F5/USD</v>
       </c>
       <c r="F36" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
-      </c>
-      <c r="G36" s="102" t="str">
+        <v>Apple_Nasdaq_AAPL</v>
+      </c>
+      <c r="G36" s="102">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
-      </c>
-      <c r="H36" s="102" t="str">
+        <v>49567</v>
+      </c>
+      <c r="H36" s="102">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
-      </c>
-      <c r="I36" s="102" t="str">
+        <v>9417730</v>
+      </c>
+      <c r="I36" s="102">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>8466043.5999999996</v>
       </c>
       <c r="J36" s="2"/>
       <c r="K36" s="49" t="s">
@@ -30714,23 +31033,23 @@
       <c r="D37" s="2"/>
       <c r="E37" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>LusidInstrumentId=LUID_S29JE7OA/USD</v>
       </c>
       <c r="F37" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
-      </c>
-      <c r="G37" s="102" t="str">
+        <v>USTreasury_2.00_2021</v>
+      </c>
+      <c r="G37" s="102">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
-      </c>
-      <c r="H37" s="102" t="str">
+        <v>121543</v>
+      </c>
+      <c r="H37" s="102">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
-      </c>
-      <c r="I37" s="102" t="str">
+        <v>12063142.75</v>
+      </c>
+      <c r="I37" s="102">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>11911214</v>
       </c>
       <c r="J37" s="2"/>
       <c r="K37" s="49" t="s">
@@ -30738,7 +31057,7 @@
       </c>
       <c r="L37" s="99">
         <f ca="1">F27</f>
-        <v>43808.419596180553</v>
+        <v>43833.390084606479</v>
       </c>
       <c r="M37" s="100"/>
       <c r="N37" s="100"/>
@@ -30752,30 +31071,30 @@
       <c r="D38" s="2"/>
       <c r="E38" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>LusidInstrumentId=LUID_E0FQLDV6/USD</v>
       </c>
       <c r="F38" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
-      </c>
-      <c r="G38" s="102" t="str">
+        <v>USTreasury_6.875_2025</v>
+      </c>
+      <c r="G38" s="102">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
-      </c>
-      <c r="H38" s="102" t="str">
+        <v>98444</v>
+      </c>
+      <c r="H38" s="102">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
-      </c>
-      <c r="I38" s="102" t="str">
+        <v>13878635.119999999</v>
+      </c>
+      <c r="I38" s="102">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>14014487.84</v>
       </c>
       <c r="J38" s="2"/>
       <c r="K38" s="49" t="s">
         <v>385</v>
       </c>
       <c r="L38" s="97" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="M38" s="98"/>
       <c r="N38" s="98"/>
@@ -30789,30 +31108,30 @@
       <c r="D39" s="2"/>
       <c r="E39" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F39" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G39" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H39" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I39" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J39" s="2"/>
       <c r="K39" s="49" t="s">
         <v>386</v>
       </c>
       <c r="L39" s="97" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="M39" s="98"/>
       <c r="N39" s="98"/>
@@ -30826,23 +31145,23 @@
       <c r="D40" s="2"/>
       <c r="E40" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F40" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G40" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H40" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I40" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J40" s="2"/>
       <c r="K40" s="49" t="s">
@@ -30861,34 +31180,34 @@
       <c r="D41" s="2"/>
       <c r="E41" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F41" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G41" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H41" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I41" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J41" s="2"/>
       <c r="K41" s="49" t="s">
         <v>388</v>
       </c>
-      <c r="L41" s="110" t="s">
+      <c r="L41" s="111" t="s">
         <v>389</v>
       </c>
-      <c r="M41" s="111"/>
-      <c r="N41" s="111"/>
-      <c r="O41" s="111"/>
+      <c r="M41" s="112"/>
+      <c r="N41" s="112"/>
+      <c r="O41" s="112"/>
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
     </row>
@@ -30898,30 +31217,30 @@
       <c r="D42" s="2"/>
       <c r="E42" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F42" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G42" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H42" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I42" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J42" s="2"/>
       <c r="K42" s="49"/>
-      <c r="L42" s="110"/>
-      <c r="M42" s="111"/>
-      <c r="N42" s="111"/>
-      <c r="O42" s="111"/>
+      <c r="L42" s="111"/>
+      <c r="M42" s="112"/>
+      <c r="N42" s="112"/>
+      <c r="O42" s="112"/>
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
     </row>
@@ -30931,30 +31250,30 @@
       <c r="D43" s="2"/>
       <c r="E43" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F43" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G43" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H43" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I43" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J43" s="2"/>
       <c r="K43" s="49"/>
-      <c r="L43" s="110"/>
-      <c r="M43" s="111"/>
-      <c r="N43" s="111"/>
-      <c r="O43" s="111"/>
+      <c r="L43" s="111"/>
+      <c r="M43" s="112"/>
+      <c r="N43" s="112"/>
+      <c r="O43" s="112"/>
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
     </row>
@@ -30964,30 +31283,30 @@
       <c r="D44" s="2"/>
       <c r="E44" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F44" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G44" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H44" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I44" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J44" s="2"/>
       <c r="K44" s="49"/>
-      <c r="L44" s="110"/>
-      <c r="M44" s="111"/>
-      <c r="N44" s="111"/>
-      <c r="O44" s="111"/>
+      <c r="L44" s="111"/>
+      <c r="M44" s="112"/>
+      <c r="N44" s="112"/>
+      <c r="O44" s="112"/>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
     </row>
@@ -30997,30 +31316,30 @@
       <c r="D45" s="2"/>
       <c r="E45" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F45" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G45" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H45" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I45" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J45" s="2"/>
       <c r="K45" s="49"/>
-      <c r="L45" s="110"/>
-      <c r="M45" s="111"/>
-      <c r="N45" s="111"/>
-      <c r="O45" s="111"/>
+      <c r="L45" s="111"/>
+      <c r="M45" s="112"/>
+      <c r="N45" s="112"/>
+      <c r="O45" s="112"/>
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
     </row>
@@ -31035,10 +31354,10 @@
       <c r="I46" s="102"/>
       <c r="J46" s="2"/>
       <c r="K46" s="49"/>
-      <c r="L46" s="110"/>
-      <c r="M46" s="111"/>
-      <c r="N46" s="111"/>
-      <c r="O46" s="111"/>
+      <c r="L46" s="111"/>
+      <c r="M46" s="112"/>
+      <c r="N46" s="112"/>
+      <c r="O46" s="112"/>
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
     </row>
@@ -31053,10 +31372,10 @@
       <c r="I47" s="102"/>
       <c r="J47" s="2"/>
       <c r="K47" s="49"/>
-      <c r="L47" s="110"/>
-      <c r="M47" s="111"/>
-      <c r="N47" s="111"/>
-      <c r="O47" s="111"/>
+      <c r="L47" s="111"/>
+      <c r="M47" s="112"/>
+      <c r="N47" s="112"/>
+      <c r="O47" s="112"/>
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
     </row>
@@ -31071,10 +31390,10 @@
       <c r="I48" s="102"/>
       <c r="J48" s="2"/>
       <c r="K48" s="49"/>
-      <c r="L48" s="110"/>
-      <c r="M48" s="111"/>
-      <c r="N48" s="111"/>
-      <c r="O48" s="111"/>
+      <c r="L48" s="111"/>
+      <c r="M48" s="112"/>
+      <c r="N48" s="112"/>
+      <c r="O48" s="112"/>
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
     </row>
@@ -31119,8 +31438,8 @@
   </sheetPr>
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J50" sqref="J50"/>
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31322,7 +31641,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="54" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F15" s="54"/>
       <c r="G15" s="54"/>
@@ -31337,7 +31656,7 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="53" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F16" s="54"/>
       <c r="G16" s="54"/>
@@ -31352,12 +31671,12 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="53" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F17" s="54"/>
       <c r="G17" s="54"/>
       <c r="K17" s="42" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="L17" s="11"/>
       <c r="M17" s="2"/>
@@ -31372,7 +31691,7 @@
       <c r="F18" s="54"/>
       <c r="G18" s="54"/>
       <c r="K18" s="42" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
@@ -31463,7 +31782,7 @@
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -31503,7 +31822,7 @@
       </c>
       <c r="L28" s="6" t="str">
         <f t="array" ref="L28:L31">_xll.flPropertiesAdd(E28:K31)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Keys</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -31519,22 +31838,22 @@
         <v>323</v>
       </c>
       <c r="G29" s="38" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H29" s="14" t="b">
         <v>0</v>
       </c>
       <c r="I29" s="38" t="s">
+        <v>413</v>
+      </c>
+      <c r="J29" s="33" t="s">
         <v>414</v>
       </c>
-      <c r="J29" s="33" t="s">
-        <v>415</v>
-      </c>
       <c r="K29" s="43" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="L29" s="103" t="str">
-        <v>#ERROR: User session not authenticated</v>
+        <v>Entity already exists</v>
       </c>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -31543,29 +31862,15 @@
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="11"/>
-      <c r="E30" s="38" t="s">
-        <v>396</v>
-      </c>
-      <c r="F30" s="21" t="s">
-        <v>323</v>
-      </c>
-      <c r="G30" s="38" t="s">
-        <v>418</v>
-      </c>
-      <c r="H30" s="14" t="b">
-        <v>0</v>
-      </c>
-      <c r="I30" s="38" t="s">
-        <v>418</v>
-      </c>
-      <c r="J30" s="33" t="s">
-        <v>415</v>
-      </c>
-      <c r="K30" s="43" t="s">
-        <v>397</v>
-      </c>
-      <c r="L30" s="103" t="str">
-        <v>#ERROR: User session not authenticated</v>
+      <c r="E30" s="38"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="43"/>
+      <c r="L30" s="103" t="e">
+        <v>#N/A</v>
       </c>
       <c r="M30" s="2"/>
       <c r="N30" s="2"/>
@@ -31581,8 +31886,8 @@
       <c r="I31" s="38"/>
       <c r="J31" s="33"/>
       <c r="K31" s="43"/>
-      <c r="L31" s="104" t="str">
-        <v>#ERROR: User session not authenticated</v>
+      <c r="L31" s="104" t="e">
+        <v>#N/A</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -31694,7 +31999,7 @@
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E39" s="11"/>
       <c r="F39" s="2"/>
@@ -31756,19 +32061,19 @@
         <v>357</v>
       </c>
       <c r="F42" s="38" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G42" s="38" t="s">
         <v>357</v>
       </c>
       <c r="H42" s="21" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I42" s="21"/>
       <c r="J42" s="33"/>
       <c r="K42" s="103" t="str">
         <f>_xll.flInstrumentsAdd(E41:J42)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>LUID_NAM9ARDX</v>
       </c>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
@@ -31796,7 +32101,7 @@
         <v>#ERROR: User session not authenticated</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
@@ -31810,16 +32115,16 @@
       <c r="B46" s="2"/>
       <c r="C46" s="11"/>
       <c r="D46" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E46" s="9" t="s">
         <v>400</v>
       </c>
-      <c r="E46" s="9" t="s">
+      <c r="F46" s="7" t="s">
         <v>401</v>
       </c>
-      <c r="F46" s="7" t="s">
+      <c r="G46" s="9" t="s">
         <v>402</v>
-      </c>
-      <c r="G46" s="9" t="s">
-        <v>403</v>
       </c>
       <c r="H46" s="9"/>
       <c r="I46" s="6"/>
@@ -31843,7 +32148,7 @@
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -31859,16 +32164,16 @@
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E49" s="9" t="s">
         <v>400</v>
       </c>
-      <c r="E49" s="9" t="s">
+      <c r="F49" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="F49" s="9" t="s">
-        <v>402</v>
-      </c>
       <c r="G49" s="92" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="H49" s="92"/>
       <c r="I49" s="9"/>
@@ -31882,7 +32187,7 @@
         <v>1</v>
       </c>
       <c r="D50" s="38" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E50" s="38" t="s">
         <v>357</v>
@@ -31895,7 +32200,7 @@
       <c r="I50" s="105"/>
       <c r="J50" s="103" t="str">
         <f>_xll.flInstrumentPropertiesAdd(D49:G50)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>OK</v>
       </c>
       <c r="K50" s="2"/>
     </row>
@@ -32009,8 +32314,8 @@
   </sheetPr>
   <dimension ref="B1:R79"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView showGridLines="0" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P68" sqref="P68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32198,7 +32503,7 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="56" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F14" s="41"/>
       <c r="G14" s="41"/>
@@ -32214,12 +32519,12 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="54" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="F15" s="54"/>
       <c r="G15" s="54"/>
       <c r="M15" s="42" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
@@ -32229,12 +32534,12 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="53" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="F16" s="54"/>
       <c r="G16" s="54"/>
       <c r="M16" s="42" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
@@ -32406,7 +32711,7 @@
       </c>
       <c r="F27" s="89">
         <f ca="1">'Upserting market quotes'!F26</f>
-        <v>43808.419596180553</v>
+        <v>43833.390084606479</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
@@ -32494,24 +32799,24 @@
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="91" t="str">
-        <f t="array" aca="1" ref="E33:I44" ca="1">_xll.flAggregatePortfolio(F23,F25,K33:L39,L40)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <f t="array" ref="E33:I44" ca="1">_xll.flAggregatePortfolio(F23,F25,K33:L39,L40)</f>
+        <v>CostSum</v>
       </c>
       <c r="F33" s="91" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>PVSum</v>
       </c>
       <c r="G33" s="91" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Name</v>
       </c>
       <c r="H33" s="91" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I33" s="91" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J33" s="2"/>
       <c r="K33" s="92" t="s">
@@ -32530,25 +32835,25 @@
       <c r="B34" s="11"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="93" t="str">
+      <c r="E34" s="93">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
-      </c>
-      <c r="F34" s="101" t="str">
+        <v>43109507.869999997</v>
+      </c>
+      <c r="F34" s="101">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>42504995.439999998</v>
       </c>
       <c r="G34" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>UKHGE base fund</v>
       </c>
       <c r="H34" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I34" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J34" s="2"/>
       <c r="K34" s="49" t="s">
@@ -32567,23 +32872,23 @@
       <c r="D35" s="2"/>
       <c r="E35" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F35" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G35" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H35" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I35" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J35" s="2"/>
       <c r="K35" s="49" t="s">
@@ -32602,23 +32907,23 @@
       <c r="D36" s="2"/>
       <c r="E36" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F36" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G36" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H36" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I36" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J36" s="2"/>
       <c r="K36" s="49" t="s">
@@ -32626,7 +32931,7 @@
       </c>
       <c r="L36" s="99">
         <f ca="1">F27</f>
-        <v>43808.419596180553</v>
+        <v>43833.390084606479</v>
       </c>
       <c r="M36" s="100"/>
       <c r="N36" s="100"/>
@@ -32640,30 +32945,30 @@
       <c r="D37" s="2"/>
       <c r="E37" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F37" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G37" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H37" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I37" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J37" s="2"/>
       <c r="K37" s="49" t="s">
         <v>385</v>
       </c>
       <c r="L37" s="97" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="M37" s="98"/>
       <c r="N37" s="98"/>
@@ -32677,30 +32982,30 @@
       <c r="D38" s="2"/>
       <c r="E38" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F38" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G38" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H38" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I38" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J38" s="2"/>
       <c r="K38" s="49" t="s">
         <v>386</v>
       </c>
       <c r="L38" s="97" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="M38" s="98"/>
       <c r="N38" s="98"/>
@@ -32714,23 +33019,23 @@
       <c r="D39" s="2"/>
       <c r="E39" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F39" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G39" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H39" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I39" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J39" s="2"/>
       <c r="K39" s="49" t="s">
@@ -32749,34 +33054,34 @@
       <c r="D40" s="2"/>
       <c r="E40" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F40" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G40" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H40" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I40" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J40" s="2"/>
       <c r="K40" s="49" t="s">
         <v>388</v>
       </c>
-      <c r="L40" s="110" t="s">
+      <c r="L40" s="111" t="s">
         <v>389</v>
       </c>
-      <c r="M40" s="111"/>
-      <c r="N40" s="111"/>
-      <c r="O40" s="111"/>
+      <c r="M40" s="112"/>
+      <c r="N40" s="112"/>
+      <c r="O40" s="112"/>
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
     </row>
@@ -32786,30 +33091,30 @@
       <c r="D41" s="2"/>
       <c r="E41" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F41" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G41" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H41" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I41" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J41" s="2"/>
       <c r="K41" s="49"/>
-      <c r="L41" s="110"/>
-      <c r="M41" s="111"/>
-      <c r="N41" s="111"/>
-      <c r="O41" s="111"/>
+      <c r="L41" s="111"/>
+      <c r="M41" s="112"/>
+      <c r="N41" s="112"/>
+      <c r="O41" s="112"/>
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
     </row>
@@ -32819,30 +33124,30 @@
       <c r="D42" s="2"/>
       <c r="E42" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F42" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G42" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H42" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I42" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J42" s="2"/>
       <c r="K42" s="49"/>
-      <c r="L42" s="110"/>
-      <c r="M42" s="111"/>
-      <c r="N42" s="111"/>
-      <c r="O42" s="111"/>
+      <c r="L42" s="111"/>
+      <c r="M42" s="112"/>
+      <c r="N42" s="112"/>
+      <c r="O42" s="112"/>
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
     </row>
@@ -32852,30 +33157,30 @@
       <c r="D43" s="2"/>
       <c r="E43" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F43" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G43" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H43" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I43" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J43" s="2"/>
       <c r="K43" s="49"/>
-      <c r="L43" s="110"/>
-      <c r="M43" s="111"/>
-      <c r="N43" s="111"/>
-      <c r="O43" s="111"/>
+      <c r="L43" s="111"/>
+      <c r="M43" s="112"/>
+      <c r="N43" s="112"/>
+      <c r="O43" s="112"/>
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
     </row>
@@ -32885,30 +33190,30 @@
       <c r="D44" s="2"/>
       <c r="E44" s="93" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="F44" s="94" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="G44" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="H44" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="I44" s="102" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v/>
       </c>
       <c r="J44" s="2"/>
       <c r="K44" s="49"/>
-      <c r="L44" s="110"/>
-      <c r="M44" s="111"/>
-      <c r="N44" s="111"/>
-      <c r="O44" s="111"/>
+      <c r="L44" s="111"/>
+      <c r="M44" s="112"/>
+      <c r="N44" s="112"/>
+      <c r="O44" s="112"/>
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
     </row>
@@ -32923,10 +33228,10 @@
       <c r="I45" s="102"/>
       <c r="J45" s="2"/>
       <c r="K45" s="49"/>
-      <c r="L45" s="110"/>
-      <c r="M45" s="111"/>
-      <c r="N45" s="111"/>
-      <c r="O45" s="111"/>
+      <c r="L45" s="111"/>
+      <c r="M45" s="112"/>
+      <c r="N45" s="112"/>
+      <c r="O45" s="112"/>
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
     </row>
@@ -32941,10 +33246,10 @@
       <c r="I46" s="102"/>
       <c r="J46" s="2"/>
       <c r="K46" s="49"/>
-      <c r="L46" s="110"/>
-      <c r="M46" s="111"/>
-      <c r="N46" s="111"/>
-      <c r="O46" s="111"/>
+      <c r="L46" s="111"/>
+      <c r="M46" s="112"/>
+      <c r="N46" s="112"/>
+      <c r="O46" s="112"/>
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
     </row>
@@ -32959,10 +33264,10 @@
       <c r="I47" s="102"/>
       <c r="J47" s="2"/>
       <c r="K47" s="49"/>
-      <c r="L47" s="110"/>
-      <c r="M47" s="111"/>
-      <c r="N47" s="111"/>
-      <c r="O47" s="111"/>
+      <c r="L47" s="111"/>
+      <c r="M47" s="112"/>
+      <c r="N47" s="112"/>
+      <c r="O47" s="112"/>
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
     </row>
@@ -33005,7 +33310,7 @@
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
@@ -33015,7 +33320,7 @@
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="F52" s="41"/>
       <c r="G52" s="108">
@@ -33034,12 +33339,12 @@
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F53" s="41"/>
-      <c r="G53" s="108" t="str">
+      <c r="G53" s="108">
         <f ca="1">F34</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>42504995.439999998</v>
       </c>
       <c r="M53" s="42"/>
       <c r="N53" s="2"/>
@@ -33050,12 +33355,12 @@
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="53" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="F54" s="54"/>
-      <c r="G54" s="54" t="e">
+      <c r="G54" s="54">
         <f ca="1">ROUND(G53/G52,2)</f>
-        <v>#VALUE!</v>
+        <v>1062.6199999999999</v>
       </c>
       <c r="M54" s="42"/>
       <c r="N54" s="2"/>
@@ -33100,7 +33405,7 @@
     <row r="58" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="60" spans="2:17" x14ac:dyDescent="0.25">
       <c r="E60" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="61" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -33170,7 +33475,7 @@
       </c>
       <c r="F64" s="74">
         <f ca="1">NOW()-4</f>
-        <v>43808.419595949075</v>
+        <v>43833.39007858796</v>
       </c>
       <c r="G64" s="55" t="s">
         <v>358</v>
@@ -33281,7 +33586,7 @@
       </c>
       <c r="H68" s="109" t="str">
         <f>'Securitising base fund'!K42</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>LUID_NAM9ARDX</v>
       </c>
       <c r="I68" s="21" t="s">
         <v>194</v>
@@ -33289,22 +33594,22 @@
       <c r="J68" s="21" t="s">
         <v>371</v>
       </c>
-      <c r="K68" s="33" t="e">
+      <c r="K68" s="33">
         <f ca="1">G54</f>
-        <v>#VALUE!</v>
+        <v>1062.6199999999999</v>
       </c>
       <c r="L68" s="43" t="s">
         <v>8</v>
       </c>
       <c r="M68" s="87">
         <f ca="1">F64</f>
-        <v>43808.419595949075</v>
+        <v>43833.39007858796</v>
       </c>
       <c r="N68" s="50"/>
       <c r="O68" s="50"/>
-      <c r="P68" s="50" t="str">
+      <c r="P68" s="103" t="str">
         <f ca="1">_xll.flQuotesAdd(F62,E67:O72)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Added 1 quote(s) as at time 2020-01-07 09:21:43Z</v>
       </c>
       <c r="Q68" s="2"/>
     </row>
@@ -33545,8 +33850,8 @@
   </sheetPr>
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33738,7 +34043,7 @@
       <c r="C13" s="55"/>
       <c r="D13" s="55"/>
       <c r="E13" s="56" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="F13" s="56"/>
       <c r="G13" s="56"/>
@@ -33768,7 +34073,7 @@
       <c r="C15" s="55"/>
       <c r="D15" s="55"/>
       <c r="E15" s="54" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="F15" s="54"/>
       <c r="G15" s="54"/>
@@ -33784,7 +34089,7 @@
       <c r="C16" s="55"/>
       <c r="D16" s="55"/>
       <c r="E16" s="54" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="F16" s="54"/>
       <c r="G16" s="54"/>
@@ -33800,7 +34105,7 @@
       <c r="C17" s="55"/>
       <c r="D17" s="55"/>
       <c r="E17" s="54" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="F17" s="54"/>
       <c r="G17" s="54"/>
@@ -34005,17 +34310,17 @@
         <v>1</v>
       </c>
       <c r="E29" s="59" t="s">
+        <v>440</v>
+      </c>
+      <c r="F29" s="58" t="s">
+        <v>441</v>
+      </c>
+      <c r="G29" s="59" t="s">
         <v>442</v>
-      </c>
-      <c r="F29" s="58" t="s">
-        <v>443</v>
-      </c>
-      <c r="G29" s="59" t="s">
-        <v>444</v>
       </c>
       <c r="H29" s="74">
         <f ca="1">NOW()-365</f>
-        <v>43447.419595949075</v>
+        <v>43472.39007858796</v>
       </c>
       <c r="I29" s="59" t="s">
         <v>14</v>
@@ -34025,9 +34330,9 @@
         <v>226</v>
       </c>
       <c r="L29" s="38"/>
-      <c r="M29" s="38" t="str">
+      <c r="M29" s="103" t="str">
         <f t="array" aca="1" ref="M29:M33" ca="1">_xll.flPortfoliosAdd(F25,E28:L33)</f>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Entity already exists</v>
       </c>
       <c r="N29" s="17"/>
     </row>
@@ -34039,17 +34344,17 @@
         <v>2</v>
       </c>
       <c r="E30" s="59" t="s">
+        <v>443</v>
+      </c>
+      <c r="F30" s="58" t="s">
+        <v>444</v>
+      </c>
+      <c r="G30" s="59" t="s">
         <v>445</v>
-      </c>
-      <c r="F30" s="58" t="s">
-        <v>446</v>
-      </c>
-      <c r="G30" s="59" t="s">
-        <v>447</v>
       </c>
       <c r="H30" s="74">
         <f ca="1">NOW()-365</f>
-        <v>43447.419595949075</v>
+        <v>43472.39007858796</v>
       </c>
       <c r="I30" s="59" t="s">
         <v>69</v>
@@ -34059,9 +34364,9 @@
         <v>226</v>
       </c>
       <c r="L30" s="35"/>
-      <c r="M30" s="38" t="str">
+      <c r="M30" s="103" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Entity already exists</v>
       </c>
       <c r="N30" s="2"/>
     </row>
@@ -34073,17 +34378,17 @@
         <v>3</v>
       </c>
       <c r="E31" s="59" t="s">
+        <v>446</v>
+      </c>
+      <c r="F31" s="58" t="s">
+        <v>447</v>
+      </c>
+      <c r="G31" s="59" t="s">
         <v>448</v>
-      </c>
-      <c r="F31" s="58" t="s">
-        <v>449</v>
-      </c>
-      <c r="G31" s="59" t="s">
-        <v>450</v>
       </c>
       <c r="H31" s="74">
         <f ca="1">NOW()-365</f>
-        <v>43447.419595949075</v>
+        <v>43472.39007858796</v>
       </c>
       <c r="I31" s="59" t="s">
         <v>8</v>
@@ -34093,9 +34398,9 @@
         <v>226</v>
       </c>
       <c r="L31" s="35"/>
-      <c r="M31" s="38" t="str">
+      <c r="M31" s="103" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Entity already exists</v>
       </c>
       <c r="N31" s="2"/>
     </row>
@@ -34107,17 +34412,17 @@
         <v>4</v>
       </c>
       <c r="E32" s="59" t="s">
+        <v>449</v>
+      </c>
+      <c r="F32" s="58" t="s">
+        <v>450</v>
+      </c>
+      <c r="G32" s="59" t="s">
         <v>451</v>
-      </c>
-      <c r="F32" s="58" t="s">
-        <v>452</v>
-      </c>
-      <c r="G32" s="59" t="s">
-        <v>453</v>
       </c>
       <c r="H32" s="74">
         <f ca="1">NOW()-365</f>
-        <v>43447.419595949075</v>
+        <v>43472.39007858796</v>
       </c>
       <c r="I32" s="59" t="s">
         <v>5</v>
@@ -34127,9 +34432,9 @@
         <v>226</v>
       </c>
       <c r="L32" s="35"/>
-      <c r="M32" s="38" t="str">
+      <c r="M32" s="103" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Entity already exists</v>
       </c>
       <c r="N32" s="2"/>
     </row>
@@ -34141,17 +34446,17 @@
         <v>5</v>
       </c>
       <c r="E33" s="59" t="s">
+        <v>452</v>
+      </c>
+      <c r="F33" s="58" t="s">
+        <v>453</v>
+      </c>
+      <c r="G33" s="59" t="s">
         <v>454</v>
-      </c>
-      <c r="F33" s="58" t="s">
-        <v>455</v>
-      </c>
-      <c r="G33" s="59" t="s">
-        <v>456</v>
       </c>
       <c r="H33" s="74">
         <f ca="1">NOW()-365</f>
-        <v>43447.419595949075</v>
+        <v>43472.39007858796</v>
       </c>
       <c r="I33" s="59" t="s">
         <v>83</v>
@@ -34161,9 +34466,9 @@
         <v>226</v>
       </c>
       <c r="L33" s="35"/>
-      <c r="M33" s="38" t="str">
+      <c r="M33" s="103" t="str">
         <f ca="1"/>
-        <v>#ERROR: User session not authenticated</v>
+        <v>Entity already exists</v>
       </c>
       <c r="N33" s="2"/>
     </row>
@@ -34362,21 +34667,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ED7FFFC81E40E242B1541D0602C582EC" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="392b4aa86b54b1b44668db5e449e18a7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="43d77729-b3b5-43d2-8eeb-4fba98ba19cc" xmlns:ns4="bfb7c3a1-8446-4cdf-8803-34a87e3df632" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="da7639e5c2e6b11c3a3b85f93dd9e28c" ns3:_="" ns4:_="">
     <xsd:import namespace="43d77729-b3b5-43d2-8eeb-4fba98ba19cc"/>
@@ -34547,10 +34837,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{806B5E61-CB82-4E98-BB90-ED4847D7777A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EE340CE-0FB2-490C-8292-BC185D93D393}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="43d77729-b3b5-43d2-8eeb-4fba98ba19cc"/>
+    <ds:schemaRef ds:uri="bfb7c3a1-8446-4cdf-8803-34a87e3df632"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -34573,20 +34889,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EE340CE-0FB2-490C-8292-BC185D93D393}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{806B5E61-CB82-4E98-BB90-ED4847D7777A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="43d77729-b3b5-43d2-8eeb-4fba98ba19cc"/>
-    <ds:schemaRef ds:uri="bfb7c3a1-8446-4cdf-8803-34a87e3df632"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>